<commit_message>
Updated UI and Status Report View
Updated UI to match specifications.
Bare Implementation but not polished Status, need to add filter, header and etc
</commit_message>
<xml_diff>
--- a/Farrowing.xlsx
+++ b/Farrowing.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="218">
   <si>
     <t>Ref. No.</t>
   </si>
@@ -335,9 +335,6 @@
     <t>08160</t>
   </si>
   <si>
-    <t>A074</t>
-  </si>
-  <si>
     <t>08984</t>
   </si>
   <si>
@@ -590,10 +587,88 @@
     <t>A124</t>
   </si>
   <si>
+    <t>09393</t>
+  </si>
+  <si>
+    <t>09397</t>
+  </si>
+  <si>
+    <t>09414</t>
+  </si>
+  <si>
+    <t>A128</t>
+  </si>
+  <si>
+    <t>A127</t>
+  </si>
+  <si>
+    <t>A126</t>
+  </si>
+  <si>
+    <t>09396</t>
+  </si>
+  <si>
+    <t>08543</t>
+  </si>
+  <si>
+    <t>09383</t>
+  </si>
+  <si>
+    <t>A129</t>
+  </si>
+  <si>
+    <t>A130</t>
+  </si>
+  <si>
+    <t>A132</t>
+  </si>
+  <si>
+    <t>08146</t>
+  </si>
+  <si>
+    <t>09374</t>
+  </si>
+  <si>
+    <t>A131</t>
+  </si>
+  <si>
+    <t>A136</t>
+  </si>
+  <si>
+    <t>A134</t>
+  </si>
+  <si>
+    <t>09390</t>
+  </si>
+  <si>
+    <t>Weaned -2 Heads Adopt(03-16-18)</t>
+  </si>
+  <si>
+    <t>Weaned - 4 Heads Adopt</t>
+  </si>
+  <si>
+    <t>Weaned +8 Heads Adopt</t>
+  </si>
+  <si>
+    <t>Weaned +5 Heads Adopt</t>
+  </si>
+  <si>
+    <t>Weaned -3 Heads Adopt</t>
+  </si>
+  <si>
+    <t>A133</t>
+  </si>
+  <si>
+    <t>09399</t>
+  </si>
+  <si>
+    <t>08988</t>
+  </si>
+  <si>
+    <t>A073</t>
+  </si>
+  <si>
     <t>0680</t>
-  </si>
-  <si>
-    <t>08988</t>
   </si>
 </sst>
 </file>
@@ -619,7 +694,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -629,6 +704,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -645,7 +726,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -661,9 +742,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -703,9 +794,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table3" displayName="Table3" ref="A1:R108" totalsRowShown="0">
-  <autoFilter ref="A1:R108">
-    <filterColumn colId="2"/>
-  </autoFilter>
+  <autoFilter ref="A1:R108"/>
   <tableColumns count="18">
     <tableColumn id="1" name="Ref. No."/>
     <tableColumn id="2" name="Farrowing Date" dataDxfId="8"/>
@@ -1018,7 +1107,7 @@
   <dimension ref="A1:R108"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44:XFD44"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1039,7 +1128,7 @@
     <col min="15" max="15" width="19.28515625" customWidth="1"/>
     <col min="16" max="16" width="15" customWidth="1"/>
     <col min="17" max="17" width="25.85546875" customWidth="1"/>
-    <col min="18" max="18" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="32.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -1151,7 +1240,7 @@
         <v>11.05</v>
       </c>
       <c r="R2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:18">
@@ -1207,7 +1296,7 @@
         <v>8.1199999999999992</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:18">
@@ -1263,53 +1352,53 @@
         <v>6.52</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:18">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="16">
         <v>43057</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="D5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="7">
+      <c r="D5" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="20">
         <v>11</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="20">
         <v>10</v>
       </c>
-      <c r="H5" s="7">
+      <c r="H5" s="20">
         <v>5</v>
       </c>
-      <c r="I5" s="7">
+      <c r="I5" s="20">
         <v>5</v>
       </c>
-      <c r="J5" s="7">
-        <v>1</v>
-      </c>
-      <c r="K5" s="7">
-        <v>0</v>
-      </c>
-      <c r="L5" s="10">
+      <c r="J5" s="20">
+        <v>1</v>
+      </c>
+      <c r="K5" s="20">
+        <v>0</v>
+      </c>
+      <c r="L5" s="21">
         <v>1.05</v>
       </c>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="10"/>
-      <c r="R5" s="13" t="s">
-        <v>148</v>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="21"/>
+      <c r="R5" s="22" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:18">
@@ -1355,7 +1444,7 @@
       <c r="P6" s="3"/>
       <c r="Q6" s="10"/>
       <c r="R6" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:18">
@@ -1411,7 +1500,7 @@
         <v>7.3</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:18">
@@ -1467,7 +1556,7 @@
         <v>7.5</v>
       </c>
       <c r="R8" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:18">
@@ -1523,7 +1612,7 @@
         <v>7.68</v>
       </c>
       <c r="R9" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:18">
@@ -1579,7 +1668,7 @@
         <v>6.8</v>
       </c>
       <c r="R10" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11" spans="1:18">
@@ -1635,7 +1724,7 @@
         <v>7.49</v>
       </c>
       <c r="R11" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:18">
@@ -1691,53 +1780,53 @@
         <v>7.22</v>
       </c>
       <c r="R12" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="13" spans="1:18">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="23">
         <v>43064</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F13" s="7">
+      <c r="D13" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="20">
         <v>9</v>
       </c>
-      <c r="G13" s="7">
+      <c r="G13" s="20">
         <v>8</v>
       </c>
-      <c r="H13" s="7">
+      <c r="H13" s="20">
         <v>3</v>
       </c>
-      <c r="I13" s="7">
+      <c r="I13" s="20">
         <v>5</v>
       </c>
-      <c r="J13" s="7">
-        <v>1</v>
-      </c>
-      <c r="K13" s="7">
-        <v>0</v>
-      </c>
-      <c r="L13" s="10">
+      <c r="J13" s="20">
+        <v>1</v>
+      </c>
+      <c r="K13" s="20">
+        <v>0</v>
+      </c>
+      <c r="L13" s="21">
         <v>1.6</v>
       </c>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
-      <c r="Q13" s="10"/>
-      <c r="R13" s="13" t="s">
-        <v>148</v>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="21"/>
+      <c r="R13" s="22" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="14" spans="1:18">
@@ -1793,7 +1882,7 @@
         <v>8.14</v>
       </c>
       <c r="R14" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:18">
@@ -1849,7 +1938,7 @@
         <v>8.1</v>
       </c>
       <c r="R15" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="16" spans="1:18">
@@ -1905,7 +1994,7 @@
         <v>7.47</v>
       </c>
       <c r="R16" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="17" spans="1:18">
@@ -1961,7 +2050,7 @@
         <v>7.06</v>
       </c>
       <c r="R17" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="18" spans="1:18">
@@ -2017,7 +2106,7 @@
         <v>8.1300000000000008</v>
       </c>
       <c r="R18" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="19" spans="1:18">
@@ -2073,7 +2162,7 @@
         <v>6.56</v>
       </c>
       <c r="R19" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="20" spans="1:18">
@@ -2090,7 +2179,7 @@
         <v>20</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>191</v>
+        <v>217</v>
       </c>
       <c r="F20" s="7">
         <v>12</v>
@@ -2129,7 +2218,7 @@
         <v>8.32</v>
       </c>
       <c r="R20" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21" spans="1:18">
@@ -2146,7 +2235,7 @@
         <v>20</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>191</v>
+        <v>217</v>
       </c>
       <c r="F21" s="7">
         <v>9</v>
@@ -2239,7 +2328,7 @@
         <v>7</v>
       </c>
       <c r="R22" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="23" spans="1:18">
@@ -2295,7 +2384,7 @@
         <v>6.96</v>
       </c>
       <c r="R23" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="24" spans="1:18">
@@ -2351,7 +2440,7 @@
         <v>9.15</v>
       </c>
       <c r="R24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="25" spans="1:18">
@@ -2407,7 +2496,7 @@
         <v>6.7</v>
       </c>
       <c r="R25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="26" spans="1:18">
@@ -2463,7 +2552,7 @@
         <v>7.52</v>
       </c>
       <c r="R26" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="27" spans="1:18">
@@ -2519,7 +2608,7 @@
         <v>10.63</v>
       </c>
       <c r="R27" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="28" spans="1:18">
@@ -2575,7 +2664,7 @@
         <v>8.02</v>
       </c>
       <c r="R28" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="29" spans="1:18">
@@ -2631,7 +2720,7 @@
         <v>7.7</v>
       </c>
       <c r="R29" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="30" spans="1:18">
@@ -2687,7 +2776,7 @@
         <v>9.07</v>
       </c>
       <c r="R30" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="31" spans="1:18">
@@ -2740,7 +2829,7 @@
         <v>31</v>
       </c>
       <c r="R31" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="32" spans="1:18">
@@ -2796,7 +2885,7 @@
         <v>8.68</v>
       </c>
       <c r="R32" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="33" spans="1:18">
@@ -2844,7 +2933,7 @@
       <c r="P33" s="3"/>
       <c r="Q33" s="3"/>
       <c r="R33" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="34" spans="1:18">
@@ -2900,7 +2989,7 @@
         <v>11.43</v>
       </c>
       <c r="R34" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="35" spans="1:18">
@@ -2956,7 +3045,7 @@
         <v>10.5</v>
       </c>
       <c r="R35" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="36" spans="1:18">
@@ -3012,7 +3101,7 @@
         <v>8.23</v>
       </c>
       <c r="R36" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="37" spans="1:18">
@@ -3068,7 +3157,7 @@
         <v>7.04</v>
       </c>
       <c r="R37" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="38" spans="1:18">
@@ -3124,7 +3213,7 @@
         <v>7.11</v>
       </c>
       <c r="R38" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="39" spans="1:18">
@@ -3180,7 +3269,7 @@
         <v>7.08</v>
       </c>
       <c r="R39" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="40" spans="1:18">
@@ -3236,7 +3325,7 @@
         <v>7.41</v>
       </c>
       <c r="R40" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="41" spans="1:18">
@@ -3292,7 +3381,7 @@
         <v>7.96</v>
       </c>
       <c r="R41" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="42" spans="1:18">
@@ -3348,18 +3437,18 @@
         <v>8.76</v>
       </c>
       <c r="R42" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="43" spans="1:18">
       <c r="A43" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B43" s="2">
         <v>43115</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D43" t="s">
         <v>20</v>
@@ -3404,12 +3493,12 @@
         <v>7.1</v>
       </c>
       <c r="R43" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="44" spans="1:18">
       <c r="A44" t="s">
-        <v>106</v>
+        <v>216</v>
       </c>
       <c r="B44" s="2">
         <v>43120</v>
@@ -3460,18 +3549,18 @@
         <v>7.59</v>
       </c>
       <c r="R44" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="45" spans="1:18">
       <c r="A45" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B45" s="2">
         <v>43124</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D45" t="s">
         <v>20</v>
@@ -3516,18 +3605,18 @@
         <v>7.58</v>
       </c>
       <c r="R45" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="46" spans="1:18">
       <c r="A46" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B46" s="2">
         <v>43125</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D46" t="s">
         <v>20</v>
@@ -3572,21 +3661,21 @@
         <v>8.4700000000000006</v>
       </c>
       <c r="R46" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="47" spans="1:18">
       <c r="A47" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B47" s="2">
         <v>43123</v>
       </c>
       <c r="C47" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D47" t="s">
         <v>157</v>
-      </c>
-      <c r="D47" t="s">
-        <v>158</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>21</v>
@@ -3628,18 +3717,18 @@
         <v>7.94</v>
       </c>
       <c r="R47" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="48" spans="1:18">
       <c r="A48" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B48" s="2">
         <v>43127</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D48" t="s">
         <v>20</v>
@@ -3684,18 +3773,18 @@
         <v>6.95</v>
       </c>
       <c r="R48" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="49" spans="1:18">
       <c r="A49" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B49" s="2">
         <v>43127</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D49" t="s">
         <v>20</v>
@@ -3740,18 +3829,18 @@
         <v>6.92</v>
       </c>
       <c r="R49" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="50" spans="1:18">
       <c r="A50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B50" s="2">
         <v>43131</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D50" t="s">
         <v>20</v>
@@ -3796,18 +3885,18 @@
         <v>9.68</v>
       </c>
       <c r="R50" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="51" spans="1:18">
       <c r="A51" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B51" s="2">
         <v>43131</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D51" t="s">
         <v>20</v>
@@ -3852,18 +3941,18 @@
         <v>8.7799999999999994</v>
       </c>
       <c r="R51" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="52" spans="1:18">
       <c r="A52" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B52" s="2">
         <v>43131</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D52" t="s">
         <v>20</v>
@@ -3908,18 +3997,18 @@
         <v>10.55</v>
       </c>
       <c r="R52" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="53" spans="1:18">
       <c r="A53" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B53" s="2">
         <v>43133</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D53" t="s">
         <v>20</v>
@@ -3964,18 +4053,18 @@
         <v>9.4</v>
       </c>
       <c r="R53" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="54" spans="1:18">
       <c r="A54" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B54" s="2">
         <v>43134</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D54" t="s">
         <v>20</v>
@@ -4020,18 +4109,18 @@
         <v>9.93</v>
       </c>
       <c r="R54" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="55" spans="1:18">
       <c r="A55" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B55" s="2">
         <v>43138</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D55" t="s">
         <v>20</v>
@@ -4076,18 +4165,18 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="R55" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="56" spans="1:18">
       <c r="A56" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B56" s="5">
         <v>43139</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>192</v>
+        <v>215</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>20</v>
@@ -4132,18 +4221,18 @@
         <v>7.78</v>
       </c>
       <c r="R56" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="57" spans="1:18">
       <c r="A57" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B57" s="2">
         <v>43140</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D57" t="s">
         <v>20</v>
@@ -4188,18 +4277,18 @@
         <v>8.07</v>
       </c>
       <c r="R57" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="58" spans="1:18">
       <c r="A58" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B58" s="2">
         <v>43142</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D58" t="s">
         <v>20</v>
@@ -4228,16 +4317,34 @@
       <c r="L58">
         <v>1.28</v>
       </c>
+      <c r="M58">
+        <v>1</v>
+      </c>
+      <c r="N58" s="8">
+        <v>43175</v>
+      </c>
+      <c r="O58">
+        <v>10</v>
+      </c>
+      <c r="P58">
+        <v>31</v>
+      </c>
+      <c r="Q58">
+        <v>8.27</v>
+      </c>
+      <c r="R58" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="59" spans="1:18">
       <c r="A59" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B59" s="2">
         <v>43138</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D59" t="s">
         <v>20</v>
@@ -4282,18 +4389,18 @@
         <v>9.44</v>
       </c>
       <c r="R59" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="60" spans="1:18">
       <c r="A60" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B60" s="2">
         <v>43142</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D60" t="s">
         <v>20</v>
@@ -4322,16 +4429,34 @@
       <c r="L60">
         <v>1.1399999999999999</v>
       </c>
+      <c r="M60">
+        <v>0</v>
+      </c>
+      <c r="N60" s="8">
+        <v>43175</v>
+      </c>
+      <c r="O60">
+        <v>10</v>
+      </c>
+      <c r="P60">
+        <v>31</v>
+      </c>
+      <c r="Q60">
+        <v>8.2200000000000006</v>
+      </c>
+      <c r="R60" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="61" spans="1:18">
       <c r="A61" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B61" s="2">
         <v>43143</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D61" t="s">
         <v>20</v>
@@ -4360,16 +4485,34 @@
       <c r="L61">
         <v>1.61</v>
       </c>
+      <c r="M61">
+        <v>2</v>
+      </c>
+      <c r="N61" s="8">
+        <v>43175</v>
+      </c>
+      <c r="O61">
+        <v>7</v>
+      </c>
+      <c r="P61">
+        <v>31</v>
+      </c>
+      <c r="Q61">
+        <v>8.7200000000000006</v>
+      </c>
+      <c r="R61" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="62" spans="1:18">
       <c r="A62" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B62" s="2">
         <v>43142</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D62" t="s">
         <v>20</v>
@@ -4398,16 +4541,34 @@
       <c r="L62">
         <v>0</v>
       </c>
+      <c r="M62">
+        <v>0</v>
+      </c>
+      <c r="N62" s="8">
+        <v>43175</v>
+      </c>
+      <c r="O62">
+        <v>8</v>
+      </c>
+      <c r="P62">
+        <v>31</v>
+      </c>
+      <c r="Q62">
+        <v>11.65</v>
+      </c>
+      <c r="R62" t="s">
+        <v>210</v>
+      </c>
     </row>
     <row r="63" spans="1:18">
       <c r="A63" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B63" s="2">
         <v>43143</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D63" t="s">
         <v>20</v>
@@ -4439,13 +4600,13 @@
     </row>
     <row r="64" spans="1:18">
       <c r="A64" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B64" s="2">
         <v>43147</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D64" t="s">
         <v>20</v>
@@ -4474,16 +4635,34 @@
       <c r="L64">
         <v>1.08</v>
       </c>
+      <c r="M64">
+        <v>0</v>
+      </c>
+      <c r="N64" s="8">
+        <v>43175</v>
+      </c>
+      <c r="O64">
+        <v>9</v>
+      </c>
+      <c r="P64">
+        <v>28</v>
+      </c>
+      <c r="Q64">
+        <v>8.24</v>
+      </c>
+      <c r="R64" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="65" spans="1:18">
       <c r="A65" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B65" s="2">
         <v>43147</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D65" t="s">
         <v>20</v>
@@ -4515,13 +4694,13 @@
     </row>
     <row r="66" spans="1:18">
       <c r="A66" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B66" s="2">
         <v>43153</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D66" t="s">
         <v>20</v>
@@ -4553,13 +4732,13 @@
     </row>
     <row r="67" spans="1:18">
       <c r="A67" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B67" s="2">
         <v>43153</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D67" t="s">
         <v>20</v>
@@ -4591,13 +4770,13 @@
     </row>
     <row r="68" spans="1:18">
       <c r="A68" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B68" s="2">
         <v>43153</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D68" t="s">
         <v>20</v>
@@ -4629,13 +4808,13 @@
     </row>
     <row r="69" spans="1:18">
       <c r="A69" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B69" s="2">
         <v>43156</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D69" t="s">
         <v>20</v>
@@ -4667,13 +4846,13 @@
     </row>
     <row r="70" spans="1:18">
       <c r="A70" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B70" s="2">
         <v>43160</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D70" t="s">
         <v>20</v>
@@ -4705,13 +4884,13 @@
     </row>
     <row r="71" spans="1:18">
       <c r="A71" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B71" s="2">
         <v>43160</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D71" t="s">
         <v>20</v>
@@ -4743,13 +4922,13 @@
     </row>
     <row r="72" spans="1:18">
       <c r="A72" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B72" s="2">
         <v>43160</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D72" t="s">
         <v>20</v>
@@ -4781,13 +4960,13 @@
     </row>
     <row r="73" spans="1:18">
       <c r="A73" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B73" s="2">
         <v>43161</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D73" t="s">
         <v>20</v>
@@ -4819,13 +4998,13 @@
     </row>
     <row r="74" spans="1:18">
       <c r="A74" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B74" s="2">
         <v>43162</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D74" t="s">
         <v>20</v>
@@ -4857,13 +5036,13 @@
     </row>
     <row r="75" spans="1:18">
       <c r="A75" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B75" s="2">
         <v>43166</v>
       </c>
-      <c r="C75" s="14" t="s">
-        <v>184</v>
+      <c r="C75" s="13" t="s">
+        <v>183</v>
       </c>
       <c r="D75" t="s">
         <v>20</v>
@@ -4895,13 +5074,13 @@
     </row>
     <row r="76" spans="1:18">
       <c r="A76" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B76" s="2">
         <v>43166</v>
       </c>
-      <c r="C76" s="14" t="s">
-        <v>185</v>
+      <c r="C76" s="13" t="s">
+        <v>184</v>
       </c>
       <c r="D76" t="s">
         <v>20</v>
@@ -4933,13 +5112,13 @@
     </row>
     <row r="77" spans="1:18">
       <c r="A77" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B77" s="2">
         <v>43166</v>
       </c>
-      <c r="C77" s="14" t="s">
-        <v>186</v>
+      <c r="C77" s="13" t="s">
+        <v>185</v>
       </c>
       <c r="D77" t="s">
         <v>20</v>
@@ -4971,18 +5150,20 @@
     </row>
     <row r="78" spans="1:18">
       <c r="A78" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B78" s="5">
         <v>43168</v>
       </c>
-      <c r="C78" s="15" t="s">
-        <v>188</v>
+      <c r="C78" s="14" t="s">
+        <v>187</v>
       </c>
       <c r="D78" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E78" s="4"/>
+      <c r="E78" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="F78" s="7">
         <v>14</v>
       </c>
@@ -5012,57 +5193,415 @@
       <c r="R78" s="3"/>
     </row>
     <row r="79" spans="1:18">
-      <c r="B79" s="2"/>
+      <c r="A79" t="s">
+        <v>193</v>
+      </c>
+      <c r="B79" s="2">
+        <v>43169</v>
+      </c>
+      <c r="C79" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="D79" t="s">
+        <v>20</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F79" s="6">
+        <v>10</v>
+      </c>
+      <c r="G79" s="6">
+        <v>10</v>
+      </c>
+      <c r="H79" s="6">
+        <v>7</v>
+      </c>
+      <c r="I79" s="6">
+        <v>3</v>
+      </c>
+      <c r="J79" s="6">
+        <v>0</v>
+      </c>
+      <c r="K79" s="6">
+        <v>0</v>
+      </c>
+      <c r="L79">
+        <v>1.36</v>
+      </c>
     </row>
     <row r="80" spans="1:18">
-      <c r="B80" s="2"/>
-    </row>
-    <row r="81" spans="2:2">
-      <c r="B81" s="2"/>
-    </row>
-    <row r="82" spans="2:2">
-      <c r="B82" s="2"/>
-    </row>
-    <row r="83" spans="2:2">
-      <c r="B83" s="2"/>
-    </row>
-    <row r="84" spans="2:2">
-      <c r="B84" s="2"/>
-    </row>
-    <row r="85" spans="2:2">
-      <c r="B85" s="2"/>
-    </row>
-    <row r="86" spans="2:2">
-      <c r="B86" s="2"/>
-    </row>
-    <row r="87" spans="2:2">
-      <c r="B87" s="2"/>
-    </row>
-    <row r="88" spans="2:2">
-      <c r="B88" s="2"/>
-    </row>
-    <row r="89" spans="2:2">
+      <c r="A80" t="s">
+        <v>194</v>
+      </c>
+      <c r="B80" s="2">
+        <v>43169</v>
+      </c>
+      <c r="C80" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="D80" t="s">
+        <v>20</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F80" s="6">
+        <v>10</v>
+      </c>
+      <c r="G80" s="6">
+        <v>10</v>
+      </c>
+      <c r="H80" s="6">
+        <v>7</v>
+      </c>
+      <c r="I80" s="6">
+        <v>3</v>
+      </c>
+      <c r="J80" s="6">
+        <v>0</v>
+      </c>
+      <c r="K80" s="6">
+        <v>0</v>
+      </c>
+      <c r="L80">
+        <v>1.54</v>
+      </c>
+    </row>
+    <row r="81" spans="1:18">
+      <c r="A81" t="s">
+        <v>195</v>
+      </c>
+      <c r="B81" s="2">
+        <v>43170</v>
+      </c>
+      <c r="C81" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="D81" t="s">
+        <v>20</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F81" s="6">
+        <v>8</v>
+      </c>
+      <c r="G81" s="6">
+        <v>0</v>
+      </c>
+      <c r="H81" s="6">
+        <v>6</v>
+      </c>
+      <c r="I81" s="6">
+        <v>2</v>
+      </c>
+      <c r="J81" s="6">
+        <v>0</v>
+      </c>
+      <c r="K81" s="6">
+        <v>0</v>
+      </c>
+      <c r="L81">
+        <v>1.23</v>
+      </c>
+    </row>
+    <row r="82" spans="1:18">
+      <c r="A82" t="s">
+        <v>199</v>
+      </c>
+      <c r="B82" s="2">
+        <v>43172</v>
+      </c>
+      <c r="C82" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="D82" t="s">
+        <v>20</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F82" s="6">
+        <v>11</v>
+      </c>
+      <c r="G82" s="6">
+        <v>5</v>
+      </c>
+      <c r="H82" s="6">
+        <v>2</v>
+      </c>
+      <c r="I82" s="6">
+        <v>3</v>
+      </c>
+      <c r="J82" s="6">
+        <v>2</v>
+      </c>
+      <c r="K82" s="6">
+        <v>4</v>
+      </c>
+      <c r="L82">
+        <v>1.48</v>
+      </c>
+    </row>
+    <row r="83" spans="1:18">
+      <c r="A83" t="s">
+        <v>200</v>
+      </c>
+      <c r="B83" s="2">
+        <v>43172</v>
+      </c>
+      <c r="C83" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="D83" t="s">
+        <v>20</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F83" s="6">
+        <v>12</v>
+      </c>
+      <c r="G83" s="6">
+        <v>11</v>
+      </c>
+      <c r="H83" s="6">
+        <v>5</v>
+      </c>
+      <c r="I83" s="6">
+        <v>6</v>
+      </c>
+      <c r="J83" s="6">
+        <v>1</v>
+      </c>
+      <c r="K83" s="6">
+        <v>0</v>
+      </c>
+      <c r="L83">
+        <v>1.21</v>
+      </c>
+    </row>
+    <row r="84" spans="1:18">
+      <c r="A84" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="B84" s="16">
+        <v>43172</v>
+      </c>
+      <c r="C84" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="D84" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="E84" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="F84" s="24">
+        <v>14</v>
+      </c>
+      <c r="G84" s="24">
+        <v>14</v>
+      </c>
+      <c r="H84" s="24">
+        <v>7</v>
+      </c>
+      <c r="I84" s="24">
+        <v>7</v>
+      </c>
+      <c r="J84" s="24">
+        <v>0</v>
+      </c>
+      <c r="K84" s="24">
+        <v>0</v>
+      </c>
+      <c r="L84" s="18">
+        <v>1.25</v>
+      </c>
+      <c r="M84" s="18"/>
+      <c r="N84" s="18"/>
+      <c r="O84" s="18"/>
+      <c r="P84" s="18"/>
+      <c r="Q84" s="18"/>
+      <c r="R84" s="25" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="85" spans="1:18">
+      <c r="A85" t="s">
+        <v>205</v>
+      </c>
+      <c r="B85" s="2">
+        <v>43173</v>
+      </c>
+      <c r="C85" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="D85" t="s">
+        <v>20</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F85" s="6">
+        <v>13</v>
+      </c>
+      <c r="G85" s="6">
+        <v>11</v>
+      </c>
+      <c r="H85" s="6">
+        <v>7</v>
+      </c>
+      <c r="I85" s="6">
+        <v>4</v>
+      </c>
+      <c r="J85" s="6">
+        <v>2</v>
+      </c>
+      <c r="K85" s="6">
+        <v>0</v>
+      </c>
+      <c r="L85">
+        <v>1.52</v>
+      </c>
+    </row>
+    <row r="86" spans="1:18">
+      <c r="A86" t="s">
+        <v>204</v>
+      </c>
+      <c r="B86" s="2">
+        <v>43173</v>
+      </c>
+      <c r="C86" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="D86" t="s">
+        <v>20</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F86" s="6">
+        <v>12</v>
+      </c>
+      <c r="G86" s="6">
+        <v>12</v>
+      </c>
+      <c r="H86" s="6">
+        <v>8</v>
+      </c>
+      <c r="I86" s="6">
+        <v>4</v>
+      </c>
+      <c r="J86" s="6">
+        <v>0</v>
+      </c>
+      <c r="K86" s="6">
+        <v>0</v>
+      </c>
+      <c r="L86" s="11">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18">
+      <c r="A87" t="s">
+        <v>206</v>
+      </c>
+      <c r="B87" s="2">
+        <v>43174</v>
+      </c>
+      <c r="C87" s="13" t="s">
+        <v>207</v>
+      </c>
+      <c r="D87" t="s">
+        <v>20</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F87" s="6">
+        <v>8</v>
+      </c>
+      <c r="G87" s="6">
+        <v>8</v>
+      </c>
+      <c r="H87" s="6">
+        <v>4</v>
+      </c>
+      <c r="I87" s="6">
+        <v>4</v>
+      </c>
+      <c r="J87" s="6">
+        <v>0</v>
+      </c>
+      <c r="K87" s="6">
+        <v>0</v>
+      </c>
+      <c r="L87" s="11">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="88" spans="1:18">
+      <c r="A88" t="s">
+        <v>213</v>
+      </c>
+      <c r="B88" s="2">
+        <v>43175</v>
+      </c>
+      <c r="C88" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="D88" t="s">
+        <v>20</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F88" s="6">
+        <v>8</v>
+      </c>
+      <c r="G88" s="6">
+        <v>7</v>
+      </c>
+      <c r="H88" s="6">
+        <v>4</v>
+      </c>
+      <c r="I88" s="6">
+        <v>3</v>
+      </c>
+      <c r="J88" s="6">
+        <v>1</v>
+      </c>
+      <c r="K88" s="6">
+        <v>0</v>
+      </c>
+      <c r="L88">
+        <v>1.55</v>
+      </c>
+    </row>
+    <row r="89" spans="1:18">
       <c r="B89" s="2"/>
     </row>
-    <row r="90" spans="2:2">
+    <row r="90" spans="1:18">
       <c r="B90" s="2"/>
     </row>
-    <row r="91" spans="2:2">
+    <row r="91" spans="1:18">
       <c r="B91" s="2"/>
     </row>
-    <row r="92" spans="2:2">
+    <row r="92" spans="1:18">
       <c r="B92" s="2"/>
     </row>
-    <row r="93" spans="2:2">
+    <row r="93" spans="1:18">
       <c r="B93" s="2"/>
     </row>
-    <row r="94" spans="2:2">
+    <row r="94" spans="1:18">
       <c r="B94" s="2"/>
     </row>
-    <row r="95" spans="2:2">
+    <row r="95" spans="1:18">
       <c r="B95" s="2"/>
     </row>
-    <row r="96" spans="2:2">
+    <row r="96" spans="1:18">
       <c r="B96" s="2"/>
     </row>
     <row r="97" spans="1:18">

</xml_diff>

<commit_message>
Dedicated Sow Record, added extra checkers checkers, fixed for new recording report
</commit_message>
<xml_diff>
--- a/Farrowing.xlsx
+++ b/Farrowing.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="336">
   <si>
     <t>Ref. No.</t>
   </si>
@@ -611,97 +611,418 @@
     <t>08543</t>
   </si>
   <si>
+    <t>A129</t>
+  </si>
+  <si>
+    <t>A130</t>
+  </si>
+  <si>
+    <t>A132</t>
+  </si>
+  <si>
+    <t>08146</t>
+  </si>
+  <si>
+    <t>09374</t>
+  </si>
+  <si>
+    <t>A131</t>
+  </si>
+  <si>
+    <t>A136</t>
+  </si>
+  <si>
+    <t>A134</t>
+  </si>
+  <si>
+    <t>09390</t>
+  </si>
+  <si>
+    <t>Weaned -2 Heads Adopt(03-16-18)</t>
+  </si>
+  <si>
+    <t>Weaned - 4 Heads Adopt</t>
+  </si>
+  <si>
+    <t>Weaned +8 Heads Adopt</t>
+  </si>
+  <si>
+    <t>Weaned +5 Heads Adopt</t>
+  </si>
+  <si>
+    <t>Weaned -3 Heads Adopt</t>
+  </si>
+  <si>
+    <t>A133</t>
+  </si>
+  <si>
+    <t>09399</t>
+  </si>
+  <si>
+    <t>08988</t>
+  </si>
+  <si>
+    <t>A073</t>
+  </si>
+  <si>
+    <t>08570</t>
+  </si>
+  <si>
+    <t>A135</t>
+  </si>
+  <si>
+    <t>0678/0694</t>
+  </si>
+  <si>
+    <t>08575</t>
+  </si>
+  <si>
+    <t>A137</t>
+  </si>
+  <si>
+    <t>09411</t>
+  </si>
+  <si>
+    <t>08982</t>
+  </si>
+  <si>
+    <t>A138</t>
+  </si>
+  <si>
+    <t>A139</t>
+  </si>
+  <si>
+    <t>0680</t>
+  </si>
+  <si>
+    <t>Weaned -4 Heads Adopt(03-23-18)</t>
+  </si>
+  <si>
+    <t>Weaned +1 Heads Adopt(02-25-18)</t>
+  </si>
+  <si>
+    <t>09403</t>
+  </si>
+  <si>
+    <t>08991</t>
+  </si>
+  <si>
+    <t>A143</t>
+  </si>
+  <si>
+    <t>A142</t>
+  </si>
+  <si>
+    <t>08990</t>
+  </si>
+  <si>
+    <t>A144</t>
+  </si>
+  <si>
+    <t>08546</t>
+  </si>
+  <si>
+    <t>A146</t>
+  </si>
+  <si>
+    <t>08555</t>
+  </si>
+  <si>
+    <t>A147</t>
+  </si>
+  <si>
+    <t>Weaned +2 Heads (03-3-18)</t>
+  </si>
+  <si>
+    <t>09407</t>
+  </si>
+  <si>
+    <t>A145</t>
+  </si>
+  <si>
+    <t>08563</t>
+  </si>
+  <si>
+    <t>A149</t>
+  </si>
+  <si>
+    <t>A153</t>
+  </si>
+  <si>
+    <t>0694</t>
+  </si>
+  <si>
+    <t>08553</t>
+  </si>
+  <si>
+    <t>Weaned -4 Heads Adopt</t>
+  </si>
+  <si>
+    <t>Cull Sow</t>
+  </si>
+  <si>
+    <t>09387</t>
+  </si>
+  <si>
+    <t>A158</t>
+  </si>
+  <si>
+    <t>09417</t>
+  </si>
+  <si>
+    <t>08545</t>
+  </si>
+  <si>
+    <t>A148</t>
+  </si>
+  <si>
+    <t>A156</t>
+  </si>
+  <si>
+    <t>09369</t>
+  </si>
+  <si>
+    <t>08565</t>
+  </si>
+  <si>
+    <t>A161</t>
+  </si>
+  <si>
+    <t>A159</t>
+  </si>
+  <si>
+    <t>08965</t>
+  </si>
+  <si>
+    <t>A152</t>
+  </si>
+  <si>
+    <t>08576</t>
+  </si>
+  <si>
+    <t>08582</t>
+  </si>
+  <si>
+    <t>A155</t>
+  </si>
+  <si>
+    <t>A160</t>
+  </si>
+  <si>
+    <t>A164</t>
+  </si>
+  <si>
+    <t>A162</t>
+  </si>
+  <si>
+    <t>08986</t>
+  </si>
+  <si>
+    <t>08157</t>
+  </si>
+  <si>
+    <t>Weaned -4 Heads Adopt (4-11-18)</t>
+  </si>
+  <si>
+    <t>Weaned -3 Heads Adopt (4-11-18)</t>
+  </si>
+  <si>
+    <t>Weaned -2 Adopt (4-11-18)</t>
+  </si>
+  <si>
+    <t>Weaned +1 Heads Adopt (03-20-18)</t>
+  </si>
+  <si>
+    <t>Weaned -2 Heads Adopt (04-11-18)</t>
+  </si>
+  <si>
+    <t>Weaned +3 Heads (4-6-18)</t>
+  </si>
+  <si>
+    <t>Weaned -4 Heads (4-6-18)</t>
+  </si>
+  <si>
+    <t>Weaned -1 Head Adopt (4-6-18)</t>
+  </si>
+  <si>
+    <t>Weaned -2 Heads Adopt (4-6-18)</t>
+  </si>
+  <si>
+    <t>09385</t>
+  </si>
+  <si>
+    <t>A173</t>
+  </si>
+  <si>
+    <t>A169</t>
+  </si>
+  <si>
+    <t>08937</t>
+  </si>
+  <si>
+    <t>08954</t>
+  </si>
+  <si>
+    <t>A172</t>
+  </si>
+  <si>
+    <t>A170</t>
+  </si>
+  <si>
     <t>09383</t>
   </si>
   <si>
-    <t>A129</t>
-  </si>
-  <si>
-    <t>A130</t>
-  </si>
-  <si>
-    <t>A132</t>
-  </si>
-  <si>
-    <t>08146</t>
-  </si>
-  <si>
-    <t>09374</t>
-  </si>
-  <si>
-    <t>A131</t>
-  </si>
-  <si>
-    <t>A136</t>
-  </si>
-  <si>
-    <t>A134</t>
-  </si>
-  <si>
-    <t>09390</t>
-  </si>
-  <si>
-    <t>Weaned -2 Heads Adopt(03-16-18)</t>
-  </si>
-  <si>
-    <t>Weaned - 4 Heads Adopt</t>
-  </si>
-  <si>
-    <t>Weaned +8 Heads Adopt</t>
-  </si>
-  <si>
-    <t>Weaned +5 Heads Adopt</t>
-  </si>
-  <si>
-    <t>Weaned -3 Heads Adopt</t>
-  </si>
-  <si>
-    <t>A133</t>
-  </si>
-  <si>
-    <t>09399</t>
-  </si>
-  <si>
-    <t>08988</t>
-  </si>
-  <si>
-    <t>A073</t>
-  </si>
-  <si>
-    <t>08570</t>
-  </si>
-  <si>
-    <t>A135</t>
-  </si>
-  <si>
-    <t>0678/0694</t>
-  </si>
-  <si>
-    <t>08575</t>
-  </si>
-  <si>
-    <t>A137</t>
-  </si>
-  <si>
-    <t>09411</t>
-  </si>
-  <si>
-    <t>08982</t>
-  </si>
-  <si>
-    <t>A138</t>
-  </si>
-  <si>
-    <t>A139</t>
-  </si>
-  <si>
-    <t>0680</t>
-  </si>
-  <si>
-    <t>Weaned -4 Heads Adopt(03-23-18)</t>
-  </si>
-  <si>
-    <t>Weaned +1 Heads Adopt(02-25-18)</t>
+    <t>08580</t>
+  </si>
+  <si>
+    <t>08995</t>
+  </si>
+  <si>
+    <t>A176</t>
+  </si>
+  <si>
+    <t>A178</t>
+  </si>
+  <si>
+    <t>A175</t>
+  </si>
+  <si>
+    <t>08971</t>
+  </si>
+  <si>
+    <t>A180</t>
+  </si>
+  <si>
+    <t>A177</t>
+  </si>
+  <si>
+    <t>09409</t>
+  </si>
+  <si>
+    <t>A183</t>
+  </si>
+  <si>
+    <t>A181</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weaned </t>
+  </si>
+  <si>
+    <t>Weaned -3 Heads Adopt (04-20-18)</t>
+  </si>
+  <si>
+    <t>Weaned-2 Heads Adopt (04-20-18)</t>
+  </si>
+  <si>
+    <t>08584</t>
+  </si>
+  <si>
+    <t>09377</t>
+  </si>
+  <si>
+    <t>A189</t>
+  </si>
+  <si>
+    <t>09398</t>
+  </si>
+  <si>
+    <t>A195</t>
+  </si>
+  <si>
+    <t>A194</t>
+  </si>
+  <si>
+    <t>08953</t>
+  </si>
+  <si>
+    <t>08960</t>
+  </si>
+  <si>
+    <t>A184</t>
+  </si>
+  <si>
+    <t>08950</t>
+  </si>
+  <si>
+    <t>A199</t>
+  </si>
+  <si>
+    <t>Weaned -2 Heads Adopt (4-27-18)</t>
+  </si>
+  <si>
+    <t>Weaned -1 Head Adopt(4-27-18)</t>
+  </si>
+  <si>
+    <t>Weaned - 7 Heads Adopt (4-27-18)</t>
+  </si>
+  <si>
+    <t>A182</t>
+  </si>
+  <si>
+    <t>A191</t>
+  </si>
+  <si>
+    <t>09379</t>
+  </si>
+  <si>
+    <t>A200</t>
+  </si>
+  <si>
+    <t>A208</t>
+  </si>
+  <si>
+    <t>A201</t>
+  </si>
+  <si>
+    <t>A202</t>
+  </si>
+  <si>
+    <t>A203</t>
+  </si>
+  <si>
+    <t>08983</t>
+  </si>
+  <si>
+    <t>A204</t>
+  </si>
+  <si>
+    <t>08586</t>
+  </si>
+  <si>
+    <t>A211</t>
+  </si>
+  <si>
+    <t>A215</t>
+  </si>
+  <si>
+    <t>09370</t>
+  </si>
+  <si>
+    <t>A209</t>
+  </si>
+  <si>
+    <t>09376</t>
+  </si>
+  <si>
+    <t>A207</t>
+  </si>
+  <si>
+    <t>08985</t>
+  </si>
+  <si>
+    <t>A220</t>
+  </si>
+  <si>
+    <t>A210</t>
+  </si>
+  <si>
+    <t>08998</t>
+  </si>
+  <si>
+    <t>08556</t>
+  </si>
+  <si>
+    <t>A214</t>
   </si>
 </sst>
 </file>
@@ -727,7 +1048,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -746,6 +1067,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -759,7 +1086,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -788,6 +1115,13 @@
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -826,8 +1160,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table3" displayName="Table3" ref="A1:R108" totalsRowShown="0">
-  <autoFilter ref="A1:R108"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table3" displayName="Table3" ref="A1:R154" totalsRowShown="0">
+  <autoFilter ref="A1:R154"/>
   <tableColumns count="18">
     <tableColumn id="1" name="Ref. No."/>
     <tableColumn id="2" name="Farrowing Date" dataDxfId="8"/>
@@ -1137,10 +1471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R108"/>
+  <dimension ref="A1:R154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F94" sqref="F94"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A142" sqref="A142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1988,7 +2322,7 @@
         <v>20</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F16" s="7">
         <v>10</v>
@@ -2044,7 +2378,7 @@
         <v>20</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F17" s="7">
         <v>15</v>
@@ -2100,7 +2434,7 @@
         <v>20</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F18" s="7">
         <v>14</v>
@@ -2212,7 +2546,7 @@
         <v>20</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F20" s="7">
         <v>12</v>
@@ -2268,7 +2602,7 @@
         <v>20</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F21" s="7">
         <v>9</v>
@@ -2961,7 +3295,9 @@
       <c r="M33" s="3">
         <v>0</v>
       </c>
-      <c r="N33" s="3"/>
+      <c r="N33" s="9">
+        <v>43126</v>
+      </c>
       <c r="O33" s="3"/>
       <c r="P33" s="3"/>
       <c r="Q33" s="3"/>
@@ -3531,7 +3867,7 @@
     </row>
     <row r="44" spans="1:18">
       <c r="A44" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B44" s="2">
         <v>43120</v>
@@ -4209,7 +4545,7 @@
         <v>43139</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>20</v>
@@ -4366,7 +4702,7 @@
         <v>8.27</v>
       </c>
       <c r="R58" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="59" spans="1:18">
@@ -4478,7 +4814,7 @@
         <v>8.2200000000000006</v>
       </c>
       <c r="R60" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="61" spans="1:18">
@@ -4534,7 +4870,7 @@
         <v>8.7200000000000006</v>
       </c>
       <c r="R61" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="62" spans="1:18">
@@ -4590,45 +4926,53 @@
         <v>11.65</v>
       </c>
       <c r="R62" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="63" spans="1:18">
-      <c r="A63" t="s">
+      <c r="A63" s="18" t="s">
         <v>143</v>
       </c>
-      <c r="B63" s="2">
+      <c r="B63" s="16">
         <v>43143</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="C63" s="19" t="s">
         <v>142</v>
       </c>
-      <c r="D63" t="s">
-        <v>20</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F63" s="6">
+      <c r="D63" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="E63" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="F63" s="24">
         <v>13</v>
       </c>
-      <c r="G63" s="6">
+      <c r="G63" s="24">
         <v>13</v>
       </c>
-      <c r="H63" s="6">
+      <c r="H63" s="24">
         <v>8</v>
       </c>
-      <c r="I63" s="6">
+      <c r="I63" s="24">
         <v>5</v>
       </c>
-      <c r="J63" s="6">
-        <v>0</v>
-      </c>
-      <c r="K63" s="6">
-        <v>0</v>
-      </c>
-      <c r="L63">
+      <c r="J63" s="24">
+        <v>0</v>
+      </c>
+      <c r="K63" s="24">
+        <v>0</v>
+      </c>
+      <c r="L63" s="18">
         <v>1.28</v>
+      </c>
+      <c r="M63" s="18"/>
+      <c r="N63" s="26"/>
+      <c r="O63" s="18"/>
+      <c r="P63" s="18"/>
+      <c r="Q63" s="27"/>
+      <c r="R63" s="25" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="64" spans="1:18">
@@ -4684,45 +5028,63 @@
         <v>8.24</v>
       </c>
       <c r="R64" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="65" spans="1:18">
-      <c r="A65" t="s">
+      <c r="A65" s="28" t="s">
         <v>152</v>
       </c>
-      <c r="B65" s="2">
+      <c r="B65" s="29">
         <v>43147</v>
       </c>
-      <c r="C65" s="1" t="s">
+      <c r="C65" s="30" t="s">
         <v>150</v>
       </c>
-      <c r="D65" t="s">
-        <v>20</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F65" s="6">
+      <c r="D65" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="E65" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="F65" s="31">
         <v>1</v>
       </c>
-      <c r="G65" s="6">
+      <c r="G65" s="31">
         <v>1</v>
       </c>
-      <c r="H65" s="6">
+      <c r="H65" s="31">
         <v>1</v>
       </c>
-      <c r="I65" s="6">
-        <v>0</v>
-      </c>
-      <c r="J65" s="6">
+      <c r="I65" s="31">
+        <v>0</v>
+      </c>
+      <c r="J65" s="31">
         <v>1</v>
       </c>
-      <c r="K65" s="6">
-        <v>0</v>
-      </c>
-      <c r="L65">
+      <c r="K65" s="31">
+        <v>0</v>
+      </c>
+      <c r="L65" s="28">
         <v>1.45</v>
+      </c>
+      <c r="M65" s="28">
+        <v>0</v>
+      </c>
+      <c r="N65" s="32">
+        <v>43158</v>
+      </c>
+      <c r="O65" s="28">
+        <v>0</v>
+      </c>
+      <c r="P65" s="28">
+        <v>25</v>
+      </c>
+      <c r="Q65" s="28">
+        <v>0</v>
+      </c>
+      <c r="R65" s="28" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="66" spans="1:18">
@@ -4834,7 +5196,7 @@
         <v>8.6199999999999992</v>
       </c>
       <c r="R67" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="68" spans="1:18">
@@ -4890,7 +5252,7 @@
         <v>8.42</v>
       </c>
       <c r="R68" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="69" spans="1:18">
@@ -4986,6 +5348,24 @@
       <c r="L70">
         <v>1.48</v>
       </c>
+      <c r="M70">
+        <v>0</v>
+      </c>
+      <c r="N70" s="8">
+        <v>43187</v>
+      </c>
+      <c r="O70">
+        <v>6</v>
+      </c>
+      <c r="P70">
+        <v>27</v>
+      </c>
+      <c r="Q70">
+        <v>8.23</v>
+      </c>
+      <c r="R70" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="71" spans="1:18">
       <c r="A71" t="s">
@@ -5024,6 +5404,24 @@
       <c r="L71">
         <v>2.1</v>
       </c>
+      <c r="M71">
+        <v>2</v>
+      </c>
+      <c r="N71" s="8">
+        <v>43182</v>
+      </c>
+      <c r="O71">
+        <v>7</v>
+      </c>
+      <c r="P71">
+        <v>30</v>
+      </c>
+      <c r="Q71">
+        <v>8.15</v>
+      </c>
+      <c r="R71" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="72" spans="1:18">
       <c r="A72" t="s">
@@ -5062,6 +5460,24 @@
       <c r="L72">
         <v>1.34</v>
       </c>
+      <c r="M72">
+        <v>0</v>
+      </c>
+      <c r="N72" s="8">
+        <v>43191</v>
+      </c>
+      <c r="O72">
+        <v>5</v>
+      </c>
+      <c r="P72">
+        <v>29</v>
+      </c>
+      <c r="Q72">
+        <v>9.8800000000000008</v>
+      </c>
+      <c r="R72" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="73" spans="1:18">
       <c r="A73" t="s">
@@ -5100,6 +5516,24 @@
       <c r="L73">
         <v>1.46</v>
       </c>
+      <c r="M73">
+        <v>0</v>
+      </c>
+      <c r="N73" s="8">
+        <v>43191</v>
+      </c>
+      <c r="O73">
+        <v>5</v>
+      </c>
+      <c r="P73">
+        <v>29</v>
+      </c>
+      <c r="Q73">
+        <v>9.36</v>
+      </c>
+      <c r="R73" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="74" spans="1:18">
       <c r="A74" t="s">
@@ -5176,6 +5610,24 @@
       <c r="L75">
         <v>1.35</v>
       </c>
+      <c r="M75">
+        <v>2</v>
+      </c>
+      <c r="N75" s="8">
+        <v>43196</v>
+      </c>
+      <c r="O75">
+        <v>5</v>
+      </c>
+      <c r="P75">
+        <v>29</v>
+      </c>
+      <c r="Q75">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="R75" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="76" spans="1:18">
       <c r="A76" t="s">
@@ -5214,6 +5666,24 @@
       <c r="L76">
         <v>1.1599999999999999</v>
       </c>
+      <c r="M76">
+        <v>0</v>
+      </c>
+      <c r="N76" s="8">
+        <v>43196</v>
+      </c>
+      <c r="O76">
+        <v>6</v>
+      </c>
+      <c r="P76">
+        <v>29</v>
+      </c>
+      <c r="Q76">
+        <v>7.68</v>
+      </c>
+      <c r="R76" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="77" spans="1:18">
       <c r="A77" t="s">
@@ -5252,6 +5722,24 @@
       <c r="L77">
         <v>1.1399999999999999</v>
       </c>
+      <c r="M77">
+        <v>0</v>
+      </c>
+      <c r="N77" s="8">
+        <v>43196</v>
+      </c>
+      <c r="O77">
+        <v>8</v>
+      </c>
+      <c r="P77">
+        <v>29</v>
+      </c>
+      <c r="Q77">
+        <v>8.17</v>
+      </c>
+      <c r="R77" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="78" spans="1:18">
       <c r="A78" t="s">
@@ -5290,12 +5778,24 @@
       <c r="L78" s="3">
         <v>1.18</v>
       </c>
-      <c r="M78" s="3"/>
-      <c r="N78" s="3"/>
-      <c r="O78" s="3"/>
-      <c r="P78" s="3"/>
-      <c r="Q78" s="3"/>
-      <c r="R78" s="3"/>
+      <c r="M78" s="3">
+        <v>2</v>
+      </c>
+      <c r="N78" s="9">
+        <v>43196</v>
+      </c>
+      <c r="O78" s="3">
+        <v>3</v>
+      </c>
+      <c r="P78" s="3">
+        <v>27</v>
+      </c>
+      <c r="Q78" s="3">
+        <v>7.66</v>
+      </c>
+      <c r="R78" s="3" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="79" spans="1:18">
       <c r="A79" t="s">
@@ -5334,6 +5834,24 @@
       <c r="L79">
         <v>1.36</v>
       </c>
+      <c r="M79">
+        <v>0</v>
+      </c>
+      <c r="N79" s="8">
+        <v>43196</v>
+      </c>
+      <c r="O79">
+        <v>4</v>
+      </c>
+      <c r="P79">
+        <v>27</v>
+      </c>
+      <c r="Q79">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="R79" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="80" spans="1:18">
       <c r="A80" t="s">
@@ -5372,6 +5890,24 @@
       <c r="L80">
         <v>1.54</v>
       </c>
+      <c r="M80">
+        <v>0</v>
+      </c>
+      <c r="N80" s="8">
+        <v>43196</v>
+      </c>
+      <c r="O80">
+        <v>10</v>
+      </c>
+      <c r="P80">
+        <v>26</v>
+      </c>
+      <c r="Q80">
+        <v>8.65</v>
+      </c>
+      <c r="R80" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="81" spans="1:18">
       <c r="A81" t="s">
@@ -5410,16 +5946,34 @@
       <c r="L81">
         <v>1.23</v>
       </c>
+      <c r="M81">
+        <v>0</v>
+      </c>
+      <c r="N81" s="8">
+        <v>43196</v>
+      </c>
+      <c r="O81">
+        <v>6</v>
+      </c>
+      <c r="P81">
+        <v>25</v>
+      </c>
+      <c r="Q81">
+        <v>8.1300000000000008</v>
+      </c>
+      <c r="R81" t="s">
+        <v>276</v>
+      </c>
     </row>
     <row r="82" spans="1:18">
       <c r="A82" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B82" s="2">
         <v>43172</v>
       </c>
       <c r="C82" s="13" t="s">
-        <v>198</v>
+        <v>284</v>
       </c>
       <c r="D82" t="s">
         <v>20</v>
@@ -5451,7 +6005,7 @@
     </row>
     <row r="83" spans="1:18">
       <c r="A83" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B83" s="2">
         <v>43172</v>
@@ -5486,10 +6040,28 @@
       <c r="L83">
         <v>1.21</v>
       </c>
+      <c r="M83">
+        <v>0</v>
+      </c>
+      <c r="N83" s="8">
+        <v>43201</v>
+      </c>
+      <c r="O83">
+        <v>7</v>
+      </c>
+      <c r="P83">
+        <v>27</v>
+      </c>
+      <c r="Q83">
+        <v>8.4</v>
+      </c>
+      <c r="R83" t="s">
+        <v>268</v>
+      </c>
     </row>
     <row r="84" spans="1:18">
       <c r="A84" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B84" s="16">
         <v>43172</v>
@@ -5535,13 +6107,13 @@
     </row>
     <row r="85" spans="1:18">
       <c r="A85" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B85" s="2">
         <v>43173</v>
       </c>
       <c r="C85" s="13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D85" t="s">
         <v>20</v>
@@ -5570,16 +6142,34 @@
       <c r="L85">
         <v>1.52</v>
       </c>
+      <c r="M85">
+        <v>2</v>
+      </c>
+      <c r="N85" s="8">
+        <v>43201</v>
+      </c>
+      <c r="O85">
+        <v>6</v>
+      </c>
+      <c r="P85">
+        <v>26</v>
+      </c>
+      <c r="Q85">
+        <v>8.23</v>
+      </c>
+      <c r="R85" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="86" spans="1:18">
       <c r="A86" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B86" s="2">
         <v>43173</v>
       </c>
       <c r="C86" s="13" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D86" t="s">
         <v>20</v>
@@ -5608,16 +6198,34 @@
       <c r="L86" s="11">
         <v>1.4</v>
       </c>
+      <c r="M86">
+        <v>1</v>
+      </c>
+      <c r="N86" s="8">
+        <v>43201</v>
+      </c>
+      <c r="O86">
+        <v>9</v>
+      </c>
+      <c r="P86">
+        <v>26</v>
+      </c>
+      <c r="Q86">
+        <v>8.1199999999999992</v>
+      </c>
+      <c r="R86" t="s">
+        <v>270</v>
+      </c>
     </row>
     <row r="87" spans="1:18">
       <c r="A87" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B87" s="2">
         <v>43174</v>
       </c>
       <c r="C87" s="13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D87" t="s">
         <v>20</v>
@@ -5646,16 +6254,34 @@
       <c r="L87" s="11">
         <v>1.7</v>
       </c>
+      <c r="M87">
+        <v>0</v>
+      </c>
+      <c r="N87" s="8">
+        <v>43201</v>
+      </c>
+      <c r="O87">
+        <v>9</v>
+      </c>
+      <c r="P87">
+        <v>25</v>
+      </c>
+      <c r="Q87">
+        <v>8.52</v>
+      </c>
+      <c r="R87" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="88" spans="1:18">
       <c r="A88" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B88" s="2">
         <v>43175</v>
       </c>
       <c r="C88" s="13" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D88" t="s">
         <v>20</v>
@@ -5684,22 +6310,40 @@
       <c r="L88">
         <v>1.55</v>
       </c>
+      <c r="M88">
+        <v>0</v>
+      </c>
+      <c r="N88" s="8">
+        <v>43201</v>
+      </c>
+      <c r="O88">
+        <v>5</v>
+      </c>
+      <c r="P88">
+        <v>25</v>
+      </c>
+      <c r="Q88">
+        <v>8.5299999999999994</v>
+      </c>
+      <c r="R88" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="89" spans="1:18">
       <c r="A89" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B89" s="2">
         <v>43178</v>
       </c>
       <c r="C89" s="13" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D89" t="s">
         <v>20</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F89" s="6">
         <v>13</v>
@@ -5722,16 +6366,34 @@
       <c r="L89">
         <v>1.45</v>
       </c>
+      <c r="M89">
+        <v>0</v>
+      </c>
+      <c r="N89" s="8">
+        <v>43210</v>
+      </c>
+      <c r="O89">
+        <v>9</v>
+      </c>
+      <c r="P89">
+        <v>29</v>
+      </c>
+      <c r="Q89">
+        <v>8.01</v>
+      </c>
+      <c r="R89" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="90" spans="1:18">
       <c r="A90" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B90" s="2">
         <v>43179</v>
       </c>
       <c r="C90" s="13" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D90" t="s">
         <v>20</v>
@@ -5760,16 +6422,34 @@
       <c r="L90">
         <v>1.35</v>
       </c>
+      <c r="M90">
+        <v>1</v>
+      </c>
+      <c r="N90" s="8">
+        <v>43210</v>
+      </c>
+      <c r="O90">
+        <v>11</v>
+      </c>
+      <c r="P90">
+        <v>39</v>
+      </c>
+      <c r="Q90">
+        <v>8.92</v>
+      </c>
+      <c r="R90" t="s">
+        <v>297</v>
+      </c>
     </row>
     <row r="91" spans="1:18">
       <c r="A91" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B91" s="2">
         <v>43181</v>
       </c>
       <c r="C91" s="13" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D91" t="s">
         <v>20</v>
@@ -5798,16 +6478,34 @@
       <c r="L91">
         <v>1.31</v>
       </c>
+      <c r="M91">
+        <v>1</v>
+      </c>
+      <c r="N91" s="8">
+        <v>43210</v>
+      </c>
+      <c r="O91">
+        <v>6</v>
+      </c>
+      <c r="P91">
+        <v>28</v>
+      </c>
+      <c r="Q91">
+        <v>7.75</v>
+      </c>
+      <c r="R91" t="s">
+        <v>297</v>
+      </c>
     </row>
     <row r="92" spans="1:18">
       <c r="A92" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B92" s="2">
         <v>43181</v>
       </c>
       <c r="C92" s="13" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D92" t="s">
         <v>20</v>
@@ -5836,71 +6534,2032 @@
       <c r="L92">
         <v>1.63</v>
       </c>
+      <c r="M92">
+        <v>0</v>
+      </c>
+      <c r="N92" s="8">
+        <v>43210</v>
+      </c>
+      <c r="O92">
+        <v>9</v>
+      </c>
+      <c r="P92">
+        <v>27</v>
+      </c>
+      <c r="Q92">
+        <v>9.64</v>
+      </c>
+      <c r="R92" t="s">
+        <v>296</v>
+      </c>
     </row>
     <row r="93" spans="1:18">
-      <c r="B93" s="2"/>
+      <c r="A93" t="s">
+        <v>230</v>
+      </c>
+      <c r="B93" s="2">
+        <v>43184</v>
+      </c>
+      <c r="C93" s="13" t="s">
+        <v>228</v>
+      </c>
+      <c r="D93" t="s">
+        <v>20</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F93" s="6">
+        <v>9</v>
+      </c>
+      <c r="G93" s="6">
+        <v>9</v>
+      </c>
+      <c r="H93" s="6">
+        <v>8</v>
+      </c>
+      <c r="I93" s="6">
+        <v>1</v>
+      </c>
+      <c r="J93" s="6">
+        <v>0</v>
+      </c>
+      <c r="K93" s="6">
+        <v>0</v>
+      </c>
+      <c r="L93">
+        <v>1.68</v>
+      </c>
+      <c r="M93">
+        <v>0</v>
+      </c>
+      <c r="N93" s="8">
+        <v>43210</v>
+      </c>
+      <c r="O93">
+        <v>8</v>
+      </c>
+      <c r="P93">
+        <v>26</v>
+      </c>
+      <c r="Q93">
+        <v>8.06</v>
+      </c>
+      <c r="R93" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="94" spans="1:18">
-      <c r="B94" s="2"/>
+      <c r="A94" t="s">
+        <v>231</v>
+      </c>
+      <c r="B94" s="2">
+        <v>43184</v>
+      </c>
+      <c r="C94" s="13" t="s">
+        <v>229</v>
+      </c>
+      <c r="D94" t="s">
+        <v>20</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F94" s="6">
+        <v>12</v>
+      </c>
+      <c r="G94" s="6">
+        <v>9</v>
+      </c>
+      <c r="H94" s="6">
+        <v>5</v>
+      </c>
+      <c r="I94" s="6">
+        <v>4</v>
+      </c>
+      <c r="J94" s="6">
+        <v>0</v>
+      </c>
+      <c r="K94" s="6">
+        <v>0</v>
+      </c>
+      <c r="L94">
+        <v>1.44</v>
+      </c>
+      <c r="M94">
+        <v>0</v>
+      </c>
+      <c r="N94" s="8">
+        <v>43210</v>
+      </c>
+      <c r="O94">
+        <v>8</v>
+      </c>
+      <c r="P94">
+        <v>26</v>
+      </c>
+      <c r="Q94" s="11">
+        <v>7.9</v>
+      </c>
+      <c r="R94" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="95" spans="1:18">
-      <c r="B95" s="2"/>
+      <c r="A95" t="s">
+        <v>233</v>
+      </c>
+      <c r="B95" s="2">
+        <v>43185</v>
+      </c>
+      <c r="C95" s="13" t="s">
+        <v>232</v>
+      </c>
+      <c r="D95" t="s">
+        <v>20</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F95" s="6">
+        <v>14</v>
+      </c>
+      <c r="G95" s="6">
+        <v>12</v>
+      </c>
+      <c r="H95" s="6">
+        <v>5</v>
+      </c>
+      <c r="I95" s="6">
+        <v>7</v>
+      </c>
+      <c r="J95" s="6">
+        <v>2</v>
+      </c>
+      <c r="K95" s="6">
+        <v>0</v>
+      </c>
+      <c r="L95">
+        <v>1.52</v>
+      </c>
+      <c r="M95">
+        <v>0</v>
+      </c>
+      <c r="N95" s="8">
+        <v>43217</v>
+      </c>
+      <c r="O95">
+        <v>10</v>
+      </c>
+      <c r="P95">
+        <v>30</v>
+      </c>
+      <c r="Q95">
+        <v>8.6300000000000008</v>
+      </c>
+      <c r="R95" t="s">
+        <v>310</v>
+      </c>
     </row>
     <row r="96" spans="1:18">
-      <c r="B96" s="2"/>
+      <c r="A96" t="s">
+        <v>235</v>
+      </c>
+      <c r="B96" s="2">
+        <v>43186</v>
+      </c>
+      <c r="C96" s="13" t="s">
+        <v>234</v>
+      </c>
+      <c r="D96" t="s">
+        <v>20</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F96" s="6">
+        <v>12</v>
+      </c>
+      <c r="G96" s="6">
+        <v>11</v>
+      </c>
+      <c r="H96" s="6">
+        <v>8</v>
+      </c>
+      <c r="I96" s="6">
+        <v>3</v>
+      </c>
+      <c r="J96" s="6">
+        <v>1</v>
+      </c>
+      <c r="K96" s="6">
+        <v>0</v>
+      </c>
+      <c r="L96">
+        <v>1.57</v>
+      </c>
+      <c r="M96">
+        <v>0</v>
+      </c>
+      <c r="N96" s="8">
+        <v>43217</v>
+      </c>
+      <c r="O96">
+        <v>10</v>
+      </c>
+      <c r="P96">
+        <v>30</v>
+      </c>
+      <c r="Q96">
+        <v>8.0399999999999991</v>
+      </c>
+      <c r="R96" t="s">
+        <v>311</v>
+      </c>
     </row>
     <row r="97" spans="1:18">
-      <c r="B97" s="2"/>
+      <c r="A97" t="s">
+        <v>237</v>
+      </c>
+      <c r="B97" s="2">
+        <v>43187</v>
+      </c>
+      <c r="C97" s="13" t="s">
+        <v>236</v>
+      </c>
+      <c r="D97" t="s">
+        <v>20</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F97" s="6">
+        <v>16</v>
+      </c>
+      <c r="G97" s="6">
+        <v>13</v>
+      </c>
+      <c r="H97" s="6">
+        <v>8</v>
+      </c>
+      <c r="I97" s="6">
+        <v>5</v>
+      </c>
+      <c r="J97" s="6">
+        <v>0</v>
+      </c>
+      <c r="K97" s="6">
+        <v>3</v>
+      </c>
+      <c r="L97" s="11">
+        <v>1.7</v>
+      </c>
+      <c r="M97">
+        <v>2</v>
+      </c>
+      <c r="N97" s="8">
+        <v>43217</v>
+      </c>
+      <c r="O97">
+        <v>11</v>
+      </c>
+      <c r="P97">
+        <v>29</v>
+      </c>
+      <c r="Q97">
+        <v>8.1</v>
+      </c>
+      <c r="R97" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="98" spans="1:18">
-      <c r="B98" s="2"/>
+      <c r="A98" t="s">
+        <v>240</v>
+      </c>
+      <c r="B98" s="2">
+        <v>43189</v>
+      </c>
+      <c r="C98" s="13" t="s">
+        <v>239</v>
+      </c>
+      <c r="D98" t="s">
+        <v>20</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F98" s="6">
+        <v>8</v>
+      </c>
+      <c r="G98" s="6">
+        <v>7</v>
+      </c>
+      <c r="H98" s="6">
+        <v>3</v>
+      </c>
+      <c r="I98" s="6">
+        <v>4</v>
+      </c>
+      <c r="J98" s="6">
+        <v>0</v>
+      </c>
+      <c r="K98" s="6">
+        <v>0</v>
+      </c>
+      <c r="L98">
+        <v>1.84</v>
+      </c>
+      <c r="M98">
+        <v>1</v>
+      </c>
+      <c r="N98" s="8">
+        <v>43217</v>
+      </c>
+      <c r="O98">
+        <v>4</v>
+      </c>
+      <c r="P98">
+        <v>27</v>
+      </c>
+      <c r="Q98">
+        <v>6.4</v>
+      </c>
+      <c r="R98" t="s">
+        <v>310</v>
+      </c>
     </row>
     <row r="99" spans="1:18">
-      <c r="B99" s="2"/>
+      <c r="A99" t="s">
+        <v>242</v>
+      </c>
+      <c r="B99" s="2">
+        <v>43191</v>
+      </c>
+      <c r="C99" s="13" t="s">
+        <v>241</v>
+      </c>
+      <c r="D99" t="s">
+        <v>20</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F99" s="6">
+        <v>16</v>
+      </c>
+      <c r="G99" s="6">
+        <v>16</v>
+      </c>
+      <c r="H99" s="6">
+        <v>7</v>
+      </c>
+      <c r="I99" s="6">
+        <v>9</v>
+      </c>
+      <c r="J99" s="6">
+        <v>0</v>
+      </c>
+      <c r="K99" s="6">
+        <v>0</v>
+      </c>
+      <c r="L99">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="M99">
+        <v>2</v>
+      </c>
+      <c r="N99" s="8">
+        <v>43217</v>
+      </c>
+      <c r="O99">
+        <v>7</v>
+      </c>
+      <c r="P99">
+        <v>27</v>
+      </c>
+      <c r="Q99">
+        <v>7.7</v>
+      </c>
+      <c r="R99" t="s">
+        <v>312</v>
+      </c>
     </row>
     <row r="100" spans="1:18">
-      <c r="B100" s="2"/>
+      <c r="A100" t="s">
+        <v>243</v>
+      </c>
+      <c r="B100" s="2">
+        <v>43192</v>
+      </c>
+      <c r="C100" s="13" t="s">
+        <v>258</v>
+      </c>
+      <c r="D100" t="s">
+        <v>20</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="F100" s="6">
+        <v>9</v>
+      </c>
+      <c r="G100" s="6">
+        <v>9</v>
+      </c>
+      <c r="H100" s="6">
+        <v>3</v>
+      </c>
+      <c r="I100" s="6">
+        <v>6</v>
+      </c>
+      <c r="J100" s="6">
+        <v>0</v>
+      </c>
+      <c r="K100" s="6">
+        <v>0</v>
+      </c>
+      <c r="L100">
+        <v>1.83</v>
+      </c>
     </row>
     <row r="101" spans="1:18">
-      <c r="B101" s="2"/>
+      <c r="A101" t="s">
+        <v>259</v>
+      </c>
+      <c r="B101" s="2">
+        <v>43192</v>
+      </c>
+      <c r="C101" s="13" t="s">
+        <v>245</v>
+      </c>
+      <c r="D101" t="s">
+        <v>20</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F101" s="6">
+        <v>5</v>
+      </c>
+      <c r="G101" s="6">
+        <v>4</v>
+      </c>
+      <c r="H101" s="6">
+        <v>3</v>
+      </c>
+      <c r="I101" s="6">
+        <v>1</v>
+      </c>
+      <c r="J101" s="6">
+        <v>1</v>
+      </c>
+      <c r="K101" s="6">
+        <v>0</v>
+      </c>
+      <c r="L101" s="11">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="102" spans="1:18">
-      <c r="B102" s="2"/>
+      <c r="A102" t="s">
+        <v>249</v>
+      </c>
+      <c r="B102" s="2">
+        <v>43193</v>
+      </c>
+      <c r="C102" s="13" t="s">
+        <v>248</v>
+      </c>
+      <c r="D102" t="s">
+        <v>20</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F102" s="6">
+        <v>11</v>
+      </c>
+      <c r="G102" s="6">
+        <v>11</v>
+      </c>
+      <c r="H102" s="6">
+        <v>6</v>
+      </c>
+      <c r="I102" s="6">
+        <v>5</v>
+      </c>
+      <c r="J102" s="6">
+        <v>0</v>
+      </c>
+      <c r="K102" s="6">
+        <v>0</v>
+      </c>
+      <c r="L102" s="11">
+        <v>1.4</v>
+      </c>
     </row>
     <row r="103" spans="1:18">
-      <c r="B103" s="2"/>
+      <c r="A103" t="s">
+        <v>252</v>
+      </c>
+      <c r="B103" s="2">
+        <v>43194</v>
+      </c>
+      <c r="C103" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="D103" t="s">
+        <v>20</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F103" s="6">
+        <v>1</v>
+      </c>
+      <c r="G103" s="6">
+        <v>1</v>
+      </c>
+      <c r="H103" s="6">
+        <v>0</v>
+      </c>
+      <c r="I103" s="6">
+        <v>1</v>
+      </c>
+      <c r="J103" s="6">
+        <v>0</v>
+      </c>
+      <c r="K103" s="6">
+        <v>0</v>
+      </c>
+      <c r="L103" s="11">
+        <v>1.7</v>
+      </c>
     </row>
     <row r="104" spans="1:18">
-      <c r="B104" s="2"/>
+      <c r="A104" t="s">
+        <v>253</v>
+      </c>
+      <c r="B104" s="2">
+        <v>43194</v>
+      </c>
+      <c r="C104" s="13" t="s">
+        <v>250</v>
+      </c>
+      <c r="D104" t="s">
+        <v>20</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F104" s="6">
+        <v>5</v>
+      </c>
+      <c r="G104" s="6">
+        <v>4</v>
+      </c>
+      <c r="H104" s="6">
+        <v>1</v>
+      </c>
+      <c r="I104" s="6">
+        <v>3</v>
+      </c>
+      <c r="J104" s="6">
+        <v>1</v>
+      </c>
+      <c r="K104" s="6">
+        <v>0</v>
+      </c>
+      <c r="L104" s="11">
+        <v>1.8</v>
+      </c>
     </row>
     <row r="105" spans="1:18">
-      <c r="B105" s="2"/>
+      <c r="A105" t="s">
+        <v>256</v>
+      </c>
+      <c r="B105" s="2">
+        <v>43195</v>
+      </c>
+      <c r="C105" s="13" t="s">
+        <v>254</v>
+      </c>
+      <c r="D105" t="s">
+        <v>20</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F105" s="6">
+        <v>13</v>
+      </c>
+      <c r="G105" s="6">
+        <v>13</v>
+      </c>
+      <c r="H105" s="6">
+        <v>1</v>
+      </c>
+      <c r="I105" s="6">
+        <v>12</v>
+      </c>
+      <c r="J105" s="6">
+        <v>0</v>
+      </c>
+      <c r="K105" s="6">
+        <v>0</v>
+      </c>
+      <c r="L105">
+        <v>1.36</v>
+      </c>
     </row>
     <row r="106" spans="1:18">
-      <c r="B106" s="2"/>
+      <c r="A106" t="s">
+        <v>257</v>
+      </c>
+      <c r="B106" s="2">
+        <v>43196</v>
+      </c>
+      <c r="C106" s="13" t="s">
+        <v>255</v>
+      </c>
+      <c r="D106" t="s">
+        <v>20</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F106" s="6">
+        <v>7</v>
+      </c>
+      <c r="G106" s="6">
+        <v>7</v>
+      </c>
+      <c r="H106" s="6">
+        <v>2</v>
+      </c>
+      <c r="I106" s="6">
+        <v>5</v>
+      </c>
+      <c r="J106" s="6">
+        <v>0</v>
+      </c>
+      <c r="K106" s="6">
+        <v>0</v>
+      </c>
+      <c r="L106">
+        <v>2.08</v>
+      </c>
     </row>
     <row r="107" spans="1:18">
-      <c r="B107" s="2"/>
+      <c r="A107" t="s">
+        <v>262</v>
+      </c>
+      <c r="B107" s="2">
+        <v>43196</v>
+      </c>
+      <c r="C107" s="13" t="s">
+        <v>260</v>
+      </c>
+      <c r="D107" t="s">
+        <v>20</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F107" s="6">
+        <v>12</v>
+      </c>
+      <c r="G107" s="6">
+        <v>12</v>
+      </c>
+      <c r="H107" s="6">
+        <v>7</v>
+      </c>
+      <c r="I107" s="6">
+        <v>5</v>
+      </c>
+      <c r="J107" s="6">
+        <v>0</v>
+      </c>
+      <c r="K107" s="6">
+        <v>0</v>
+      </c>
+      <c r="L107">
+        <v>1.84</v>
+      </c>
     </row>
     <row r="108" spans="1:18">
-      <c r="A108" s="3"/>
-      <c r="B108" s="5"/>
-      <c r="C108" s="4"/>
-      <c r="D108" s="3"/>
-      <c r="E108" s="4"/>
-      <c r="F108" s="7"/>
-      <c r="G108" s="7"/>
-      <c r="H108" s="7"/>
-      <c r="I108" s="7"/>
-      <c r="J108" s="7"/>
-      <c r="K108" s="7"/>
-      <c r="L108" s="3"/>
+      <c r="A108" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="B108" s="5">
+        <v>43197</v>
+      </c>
+      <c r="C108" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="D108" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E108" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F108" s="7">
+        <v>8</v>
+      </c>
+      <c r="G108" s="7">
+        <v>6</v>
+      </c>
+      <c r="H108" s="7">
+        <v>4</v>
+      </c>
+      <c r="I108" s="7">
+        <v>2</v>
+      </c>
+      <c r="J108" s="7">
+        <v>2</v>
+      </c>
+      <c r="K108" s="7">
+        <v>0</v>
+      </c>
+      <c r="L108" s="3">
+        <v>1.85</v>
+      </c>
       <c r="M108" s="3"/>
       <c r="N108" s="3"/>
       <c r="O108" s="3"/>
       <c r="P108" s="3"/>
       <c r="Q108" s="3"/>
       <c r="R108" s="3"/>
+    </row>
+    <row r="109" spans="1:18">
+      <c r="A109" t="s">
+        <v>264</v>
+      </c>
+      <c r="B109" s="2">
+        <v>43198</v>
+      </c>
+      <c r="C109" s="13" t="s">
+        <v>266</v>
+      </c>
+      <c r="D109" t="s">
+        <v>20</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F109" s="6">
+        <v>8</v>
+      </c>
+      <c r="G109" s="6">
+        <v>8</v>
+      </c>
+      <c r="H109" s="6">
+        <v>4</v>
+      </c>
+      <c r="I109" s="6">
+        <v>4</v>
+      </c>
+      <c r="J109" s="6">
+        <v>0</v>
+      </c>
+      <c r="K109" s="6">
+        <v>0</v>
+      </c>
+      <c r="L109">
+        <v>2.11</v>
+      </c>
+    </row>
+    <row r="110" spans="1:18">
+      <c r="A110" t="s">
+        <v>265</v>
+      </c>
+      <c r="B110" s="2">
+        <v>43198</v>
+      </c>
+      <c r="C110" s="13" t="s">
+        <v>267</v>
+      </c>
+      <c r="D110" t="s">
+        <v>20</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="F110" s="6">
+        <v>6</v>
+      </c>
+      <c r="G110" s="6">
+        <v>5</v>
+      </c>
+      <c r="H110" s="6">
+        <v>4</v>
+      </c>
+      <c r="I110" s="6">
+        <v>1</v>
+      </c>
+      <c r="J110" s="6">
+        <v>1</v>
+      </c>
+      <c r="K110" s="6">
+        <v>0</v>
+      </c>
+      <c r="L110">
+        <v>2.16</v>
+      </c>
+    </row>
+    <row r="111" spans="1:18">
+      <c r="A111" t="s">
+        <v>278</v>
+      </c>
+      <c r="B111" s="2">
+        <v>43202</v>
+      </c>
+      <c r="C111" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D111" t="s">
+        <v>20</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F111" s="6">
+        <v>16</v>
+      </c>
+      <c r="G111" s="6">
+        <v>13</v>
+      </c>
+      <c r="H111" s="6">
+        <v>7</v>
+      </c>
+      <c r="I111" s="6">
+        <v>6</v>
+      </c>
+      <c r="J111" s="6">
+        <v>3</v>
+      </c>
+      <c r="K111" s="6">
+        <v>0</v>
+      </c>
+      <c r="L111">
+        <v>1.88</v>
+      </c>
+    </row>
+    <row r="112" spans="1:18">
+      <c r="A112" t="s">
+        <v>279</v>
+      </c>
+      <c r="B112" s="2">
+        <v>43202</v>
+      </c>
+      <c r="C112" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="D112" t="s">
+        <v>20</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="F112" s="6">
+        <v>13</v>
+      </c>
+      <c r="G112" s="6">
+        <v>13</v>
+      </c>
+      <c r="H112" s="6">
+        <v>4</v>
+      </c>
+      <c r="I112" s="6">
+        <v>9</v>
+      </c>
+      <c r="J112" s="6">
+        <v>0</v>
+      </c>
+      <c r="K112" s="6">
+        <v>0</v>
+      </c>
+      <c r="L112">
+        <v>1.35</v>
+      </c>
+    </row>
+    <row r="113" spans="1:18">
+      <c r="A113" t="s">
+        <v>282</v>
+      </c>
+      <c r="B113" s="2">
+        <v>43202</v>
+      </c>
+      <c r="C113" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="D113" t="s">
+        <v>20</v>
+      </c>
+      <c r="E113" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F113" s="6">
+        <v>5</v>
+      </c>
+      <c r="G113" s="6">
+        <v>5</v>
+      </c>
+      <c r="H113" s="6">
+        <v>0</v>
+      </c>
+      <c r="I113" s="6">
+        <v>5</v>
+      </c>
+      <c r="J113" s="6">
+        <v>0</v>
+      </c>
+      <c r="K113" s="6">
+        <v>0</v>
+      </c>
+      <c r="L113">
+        <v>1.66</v>
+      </c>
+    </row>
+    <row r="114" spans="1:18">
+      <c r="A114" t="s">
+        <v>283</v>
+      </c>
+      <c r="B114" s="2">
+        <v>43203</v>
+      </c>
+      <c r="C114" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="D114" t="s">
+        <v>20</v>
+      </c>
+      <c r="E114" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="F114" s="6">
+        <v>8</v>
+      </c>
+      <c r="G114" s="6">
+        <v>8</v>
+      </c>
+      <c r="H114" s="6">
+        <v>4</v>
+      </c>
+      <c r="I114" s="6">
+        <v>4</v>
+      </c>
+      <c r="J114" s="6">
+        <v>0</v>
+      </c>
+      <c r="K114" s="6">
+        <v>0</v>
+      </c>
+      <c r="L114">
+        <v>2.0099999999999998</v>
+      </c>
+    </row>
+    <row r="115" spans="1:18">
+      <c r="A115" t="s">
+        <v>287</v>
+      </c>
+      <c r="B115" s="2">
+        <v>43204</v>
+      </c>
+      <c r="C115" s="13" t="s">
+        <v>285</v>
+      </c>
+      <c r="D115" t="s">
+        <v>20</v>
+      </c>
+      <c r="E115" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="F115" s="6">
+        <v>14</v>
+      </c>
+      <c r="G115" s="6">
+        <v>14</v>
+      </c>
+      <c r="H115" s="6">
+        <v>8</v>
+      </c>
+      <c r="I115" s="6">
+        <v>6</v>
+      </c>
+      <c r="J115" s="6">
+        <v>0</v>
+      </c>
+      <c r="K115" s="6">
+        <v>0</v>
+      </c>
+      <c r="L115">
+        <v>1.62</v>
+      </c>
+    </row>
+    <row r="116" spans="1:18">
+      <c r="A116" t="s">
+        <v>288</v>
+      </c>
+      <c r="B116" s="2">
+        <v>43206</v>
+      </c>
+      <c r="C116" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D116" t="s">
+        <v>20</v>
+      </c>
+      <c r="E116" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="F116" s="6">
+        <v>13</v>
+      </c>
+      <c r="G116" s="6">
+        <v>11</v>
+      </c>
+      <c r="H116" s="6">
+        <v>5</v>
+      </c>
+      <c r="I116" s="6">
+        <v>6</v>
+      </c>
+      <c r="J116" s="6">
+        <v>2</v>
+      </c>
+      <c r="K116" s="6">
+        <v>0</v>
+      </c>
+      <c r="L116">
+        <v>1.42</v>
+      </c>
+    </row>
+    <row r="117" spans="1:18">
+      <c r="A117" t="s">
+        <v>289</v>
+      </c>
+      <c r="B117" s="2">
+        <v>43206</v>
+      </c>
+      <c r="C117" s="13" t="s">
+        <v>286</v>
+      </c>
+      <c r="D117" t="s">
+        <v>20</v>
+      </c>
+      <c r="E117" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="F117" s="6">
+        <v>16</v>
+      </c>
+      <c r="G117" s="6">
+        <v>13</v>
+      </c>
+      <c r="H117" s="6">
+        <v>5</v>
+      </c>
+      <c r="I117" s="6">
+        <v>8</v>
+      </c>
+      <c r="J117" s="6">
+        <v>3</v>
+      </c>
+      <c r="K117" s="6">
+        <v>0</v>
+      </c>
+      <c r="L117">
+        <v>1.62</v>
+      </c>
+    </row>
+    <row r="118" spans="1:18">
+      <c r="A118" t="s">
+        <v>291</v>
+      </c>
+      <c r="B118" s="2">
+        <v>43207</v>
+      </c>
+      <c r="C118" s="13" t="s">
+        <v>290</v>
+      </c>
+      <c r="D118" t="s">
+        <v>20</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F118" s="6">
+        <v>8</v>
+      </c>
+      <c r="G118" s="6">
+        <v>8</v>
+      </c>
+      <c r="H118" s="6">
+        <v>5</v>
+      </c>
+      <c r="I118" s="6">
+        <v>3</v>
+      </c>
+      <c r="J118" s="6">
+        <v>0</v>
+      </c>
+      <c r="K118" s="6">
+        <v>0</v>
+      </c>
+      <c r="L118">
+        <v>1.77</v>
+      </c>
+    </row>
+    <row r="119" spans="1:18">
+      <c r="A119" t="s">
+        <v>292</v>
+      </c>
+      <c r="B119" s="2">
+        <v>43208</v>
+      </c>
+      <c r="C119" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D119" t="s">
+        <v>20</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="F119" s="6">
+        <v>9</v>
+      </c>
+      <c r="G119" s="6">
+        <v>8</v>
+      </c>
+      <c r="H119" s="6">
+        <v>3</v>
+      </c>
+      <c r="I119" s="6">
+        <v>5</v>
+      </c>
+      <c r="J119" s="6">
+        <v>1</v>
+      </c>
+      <c r="K119" s="6">
+        <v>0</v>
+      </c>
+      <c r="L119">
+        <v>2.06</v>
+      </c>
+    </row>
+    <row r="120" spans="1:18">
+      <c r="A120" t="s">
+        <v>294</v>
+      </c>
+      <c r="B120" s="2">
+        <v>43208</v>
+      </c>
+      <c r="C120" s="13" t="s">
+        <v>293</v>
+      </c>
+      <c r="D120" t="s">
+        <v>20</v>
+      </c>
+      <c r="E120" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="F120" s="6">
+        <v>5</v>
+      </c>
+      <c r="G120" s="6">
+        <v>5</v>
+      </c>
+      <c r="H120" s="6">
+        <v>5</v>
+      </c>
+      <c r="I120" s="6">
+        <v>0</v>
+      </c>
+      <c r="J120" s="6">
+        <v>0</v>
+      </c>
+      <c r="K120" s="6">
+        <v>0</v>
+      </c>
+      <c r="L120">
+        <v>1.48</v>
+      </c>
+    </row>
+    <row r="121" spans="1:18">
+      <c r="A121" t="s">
+        <v>295</v>
+      </c>
+      <c r="B121" s="2">
+        <v>43208</v>
+      </c>
+      <c r="C121" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D121" t="s">
+        <v>20</v>
+      </c>
+      <c r="E121" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="F121" s="6">
+        <v>9</v>
+      </c>
+      <c r="G121" s="6">
+        <v>9</v>
+      </c>
+      <c r="H121" s="6">
+        <v>4</v>
+      </c>
+      <c r="I121" s="6">
+        <v>5</v>
+      </c>
+      <c r="J121" s="6">
+        <v>0</v>
+      </c>
+      <c r="K121" s="6">
+        <v>0</v>
+      </c>
+      <c r="L121">
+        <v>2.33</v>
+      </c>
+    </row>
+    <row r="122" spans="1:18">
+      <c r="A122" t="s">
+        <v>301</v>
+      </c>
+      <c r="B122" s="2">
+        <v>43211</v>
+      </c>
+      <c r="C122" s="13" t="s">
+        <v>299</v>
+      </c>
+      <c r="D122" t="s">
+        <v>20</v>
+      </c>
+      <c r="E122" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F122" s="6">
+        <v>4</v>
+      </c>
+      <c r="G122" s="6">
+        <v>3</v>
+      </c>
+      <c r="H122" s="6">
+        <v>1</v>
+      </c>
+      <c r="I122" s="6">
+        <v>2</v>
+      </c>
+      <c r="J122" s="6">
+        <v>1</v>
+      </c>
+      <c r="K122" s="6">
+        <v>0</v>
+      </c>
+      <c r="L122">
+        <v>1.43</v>
+      </c>
+    </row>
+    <row r="123" spans="1:18">
+      <c r="A123" t="s">
+        <v>314</v>
+      </c>
+      <c r="B123" s="2">
+        <v>43212</v>
+      </c>
+      <c r="C123" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D123" t="s">
+        <v>20</v>
+      </c>
+      <c r="E123" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="F123" s="6">
+        <v>8</v>
+      </c>
+      <c r="G123" s="6">
+        <v>6</v>
+      </c>
+      <c r="H123" s="6">
+        <v>5</v>
+      </c>
+      <c r="I123" s="6">
+        <v>1</v>
+      </c>
+      <c r="J123" s="6">
+        <v>2</v>
+      </c>
+      <c r="K123" s="6">
+        <v>0</v>
+      </c>
+      <c r="L123">
+        <v>1.61</v>
+      </c>
+    </row>
+    <row r="124" spans="1:18">
+      <c r="A124" t="s">
+        <v>313</v>
+      </c>
+      <c r="B124" s="2">
+        <v>43212</v>
+      </c>
+      <c r="C124" s="13" t="s">
+        <v>300</v>
+      </c>
+      <c r="D124" t="s">
+        <v>20</v>
+      </c>
+      <c r="E124" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="F124" s="6">
+        <v>8</v>
+      </c>
+      <c r="G124" s="6">
+        <v>6</v>
+      </c>
+      <c r="H124" s="6">
+        <v>4</v>
+      </c>
+      <c r="I124" s="6">
+        <v>2</v>
+      </c>
+      <c r="J124" s="6">
+        <v>2</v>
+      </c>
+      <c r="K124" s="6">
+        <v>0</v>
+      </c>
+      <c r="L124">
+        <v>1.36</v>
+      </c>
+    </row>
+    <row r="125" spans="1:18">
+      <c r="A125" t="s">
+        <v>303</v>
+      </c>
+      <c r="B125" s="2">
+        <v>43215</v>
+      </c>
+      <c r="C125" s="13" t="s">
+        <v>302</v>
+      </c>
+      <c r="D125" t="s">
+        <v>20</v>
+      </c>
+      <c r="E125" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F125" s="6">
+        <v>13</v>
+      </c>
+      <c r="G125" s="6">
+        <v>12</v>
+      </c>
+      <c r="H125" s="6">
+        <v>9</v>
+      </c>
+      <c r="I125" s="6">
+        <v>3</v>
+      </c>
+      <c r="J125" s="6">
+        <v>1</v>
+      </c>
+      <c r="K125" s="6">
+        <v>0</v>
+      </c>
+      <c r="L125">
+        <v>1.43</v>
+      </c>
+    </row>
+    <row r="126" spans="1:18">
+      <c r="A126" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="B126" s="5">
+        <v>43217</v>
+      </c>
+      <c r="C126" s="14" t="s">
+        <v>305</v>
+      </c>
+      <c r="D126" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E126" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="F126" s="7">
+        <v>14</v>
+      </c>
+      <c r="G126" s="7">
+        <v>14</v>
+      </c>
+      <c r="H126" s="7">
+        <v>5</v>
+      </c>
+      <c r="I126" s="7">
+        <v>9</v>
+      </c>
+      <c r="J126" s="7">
+        <v>0</v>
+      </c>
+      <c r="K126" s="7">
+        <v>0</v>
+      </c>
+      <c r="L126" s="3">
+        <v>1.27</v>
+      </c>
+      <c r="M126" s="3"/>
+      <c r="N126" s="3"/>
+      <c r="O126" s="3"/>
+      <c r="P126" s="3"/>
+      <c r="Q126" s="3"/>
+      <c r="R126" s="3"/>
+    </row>
+    <row r="127" spans="1:18">
+      <c r="A127" t="s">
+        <v>307</v>
+      </c>
+      <c r="B127" s="2">
+        <v>43217</v>
+      </c>
+      <c r="C127" s="13" t="s">
+        <v>306</v>
+      </c>
+      <c r="D127" t="s">
+        <v>20</v>
+      </c>
+      <c r="E127" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="F127" s="6">
+        <v>3</v>
+      </c>
+      <c r="G127" s="6">
+        <v>2</v>
+      </c>
+      <c r="H127" s="6">
+        <v>1</v>
+      </c>
+      <c r="I127" s="6">
+        <v>1</v>
+      </c>
+      <c r="J127" s="6">
+        <v>1</v>
+      </c>
+      <c r="K127" s="6">
+        <v>0</v>
+      </c>
+      <c r="L127" s="11">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="128" spans="1:18">
+      <c r="A128" t="s">
+        <v>309</v>
+      </c>
+      <c r="B128" s="2">
+        <v>43217</v>
+      </c>
+      <c r="C128" s="13" t="s">
+        <v>308</v>
+      </c>
+      <c r="D128" t="s">
+        <v>20</v>
+      </c>
+      <c r="E128" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="F128" s="6">
+        <v>14</v>
+      </c>
+      <c r="G128" s="6">
+        <v>14</v>
+      </c>
+      <c r="H128" s="6">
+        <v>11</v>
+      </c>
+      <c r="I128" s="6">
+        <v>3</v>
+      </c>
+      <c r="J128" s="6">
+        <v>0</v>
+      </c>
+      <c r="K128" s="6">
+        <v>0</v>
+      </c>
+      <c r="L128" s="11">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="129" spans="1:12">
+      <c r="A129" t="s">
+        <v>316</v>
+      </c>
+      <c r="B129" s="2">
+        <v>43218</v>
+      </c>
+      <c r="C129" s="13" t="s">
+        <v>321</v>
+      </c>
+      <c r="D129" t="s">
+        <v>20</v>
+      </c>
+      <c r="E129" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="F129" s="6">
+        <v>12</v>
+      </c>
+      <c r="G129" s="6">
+        <v>12</v>
+      </c>
+      <c r="H129" s="6">
+        <v>5</v>
+      </c>
+      <c r="I129" s="6">
+        <v>7</v>
+      </c>
+      <c r="J129" s="6">
+        <v>0</v>
+      </c>
+      <c r="K129" s="6">
+        <v>0</v>
+      </c>
+      <c r="L129" s="11">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="130" spans="1:12">
+      <c r="A130" t="s">
+        <v>317</v>
+      </c>
+      <c r="B130" s="2">
+        <v>43219</v>
+      </c>
+      <c r="C130" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D130" t="s">
+        <v>20</v>
+      </c>
+      <c r="E130" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="F130" s="6">
+        <v>10</v>
+      </c>
+      <c r="G130" s="6">
+        <v>10</v>
+      </c>
+      <c r="H130" s="6">
+        <v>7</v>
+      </c>
+      <c r="I130" s="6">
+        <v>3</v>
+      </c>
+      <c r="J130" s="6">
+        <v>0</v>
+      </c>
+      <c r="K130" s="6">
+        <v>0</v>
+      </c>
+      <c r="L130">
+        <v>1.79</v>
+      </c>
+    </row>
+    <row r="131" spans="1:12">
+      <c r="A131" t="s">
+        <v>318</v>
+      </c>
+      <c r="B131" s="2">
+        <v>43219</v>
+      </c>
+      <c r="C131" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="D131" t="s">
+        <v>20</v>
+      </c>
+      <c r="E131" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="F131" s="6">
+        <v>10</v>
+      </c>
+      <c r="G131" s="6">
+        <v>7</v>
+      </c>
+      <c r="H131" s="6">
+        <v>4</v>
+      </c>
+      <c r="I131" s="6">
+        <v>3</v>
+      </c>
+      <c r="J131" s="6">
+        <v>0</v>
+      </c>
+      <c r="K131" s="6">
+        <v>0</v>
+      </c>
+      <c r="L131">
+        <v>1.22</v>
+      </c>
+    </row>
+    <row r="132" spans="1:12">
+      <c r="A132" t="s">
+        <v>319</v>
+      </c>
+      <c r="B132" s="2">
+        <v>43219</v>
+      </c>
+      <c r="C132" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D132" t="s">
+        <v>20</v>
+      </c>
+      <c r="E132" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="F132" s="6">
+        <v>11</v>
+      </c>
+      <c r="G132" s="6">
+        <v>11</v>
+      </c>
+      <c r="H132" s="6">
+        <v>3</v>
+      </c>
+      <c r="I132" s="6">
+        <v>8</v>
+      </c>
+      <c r="J132" s="6">
+        <v>0</v>
+      </c>
+      <c r="K132" s="6">
+        <v>0</v>
+      </c>
+      <c r="L132">
+        <v>1.45</v>
+      </c>
+    </row>
+    <row r="133" spans="1:12">
+      <c r="A133" t="s">
+        <v>320</v>
+      </c>
+      <c r="B133" s="2">
+        <v>43220</v>
+      </c>
+      <c r="C133" s="13" t="s">
+        <v>315</v>
+      </c>
+      <c r="D133" t="s">
+        <v>20</v>
+      </c>
+      <c r="E133" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="F133" s="6">
+        <v>14</v>
+      </c>
+      <c r="G133" s="6">
+        <v>11</v>
+      </c>
+      <c r="H133" s="6">
+        <v>7</v>
+      </c>
+      <c r="I133" s="6">
+        <v>4</v>
+      </c>
+      <c r="J133" s="6">
+        <v>3</v>
+      </c>
+      <c r="K133" s="6">
+        <v>0</v>
+      </c>
+      <c r="L133">
+        <v>1.37</v>
+      </c>
+    </row>
+    <row r="134" spans="1:12">
+      <c r="A134" t="s">
+        <v>322</v>
+      </c>
+      <c r="B134" s="2">
+        <v>43221</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="F134" s="6">
+        <v>14</v>
+      </c>
+      <c r="G134" s="6">
+        <v>12</v>
+      </c>
+      <c r="H134" s="6">
+        <v>7</v>
+      </c>
+      <c r="I134" s="6">
+        <v>5</v>
+      </c>
+      <c r="J134" s="6">
+        <v>2</v>
+      </c>
+      <c r="K134" s="6">
+        <v>0</v>
+      </c>
+      <c r="L134">
+        <v>1.31</v>
+      </c>
+    </row>
+    <row r="135" spans="1:12">
+      <c r="A135" t="s">
+        <v>324</v>
+      </c>
+      <c r="B135" s="2">
+        <v>43221</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F135" s="6">
+        <v>17</v>
+      </c>
+      <c r="G135" s="6">
+        <v>12</v>
+      </c>
+      <c r="H135" s="6">
+        <v>6</v>
+      </c>
+      <c r="I135" s="6">
+        <v>6</v>
+      </c>
+      <c r="J135" s="6">
+        <v>5</v>
+      </c>
+      <c r="K135" s="6">
+        <v>0</v>
+      </c>
+      <c r="L135">
+        <v>1.35</v>
+      </c>
+    </row>
+    <row r="136" spans="1:12">
+      <c r="A136" t="s">
+        <v>325</v>
+      </c>
+      <c r="B136" s="2">
+        <v>43222</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="F136" s="6">
+        <v>14</v>
+      </c>
+      <c r="G136" s="6">
+        <v>14</v>
+      </c>
+      <c r="H136" s="6">
+        <v>6</v>
+      </c>
+      <c r="I136" s="6">
+        <v>8</v>
+      </c>
+      <c r="J136" s="6">
+        <v>0</v>
+      </c>
+      <c r="K136" s="6">
+        <v>0</v>
+      </c>
+      <c r="L136">
+        <v>1.57</v>
+      </c>
+    </row>
+    <row r="137" spans="1:12">
+      <c r="A137" t="s">
+        <v>327</v>
+      </c>
+      <c r="B137" s="2">
+        <v>43222</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="F137" s="6">
+        <v>10</v>
+      </c>
+      <c r="G137" s="6">
+        <v>10</v>
+      </c>
+      <c r="H137" s="6">
+        <v>7</v>
+      </c>
+      <c r="I137" s="6">
+        <v>3</v>
+      </c>
+      <c r="J137" s="6">
+        <v>0</v>
+      </c>
+      <c r="K137" s="6">
+        <v>0</v>
+      </c>
+      <c r="L137">
+        <v>1.42</v>
+      </c>
+    </row>
+    <row r="138" spans="1:12">
+      <c r="A138" t="s">
+        <v>329</v>
+      </c>
+      <c r="B138" s="2">
+        <v>43222</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="F138" s="6">
+        <v>4</v>
+      </c>
+      <c r="G138" s="6">
+        <v>4</v>
+      </c>
+      <c r="H138" s="6">
+        <v>2</v>
+      </c>
+      <c r="I138" s="6">
+        <v>2</v>
+      </c>
+      <c r="J138" s="6">
+        <v>0</v>
+      </c>
+      <c r="K138" s="6">
+        <v>0</v>
+      </c>
+      <c r="L138">
+        <v>2.4500000000000002</v>
+      </c>
+    </row>
+    <row r="139" spans="1:12">
+      <c r="A139" t="s">
+        <v>331</v>
+      </c>
+      <c r="B139" s="2">
+        <v>43224</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="F139" s="6">
+        <v>11</v>
+      </c>
+      <c r="G139" s="6">
+        <v>8</v>
+      </c>
+      <c r="H139" s="6">
+        <v>6</v>
+      </c>
+      <c r="I139" s="6">
+        <v>2</v>
+      </c>
+      <c r="J139" s="6">
+        <v>3</v>
+      </c>
+      <c r="K139" s="6">
+        <v>0</v>
+      </c>
+      <c r="L139">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="140" spans="1:12">
+      <c r="A140" t="s">
+        <v>332</v>
+      </c>
+      <c r="B140" s="2">
+        <v>43224</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="F140" s="6">
+        <v>13</v>
+      </c>
+      <c r="G140" s="6">
+        <v>12</v>
+      </c>
+      <c r="H140" s="6">
+        <v>5</v>
+      </c>
+      <c r="I140" s="6">
+        <v>7</v>
+      </c>
+      <c r="J140" s="6">
+        <v>1</v>
+      </c>
+      <c r="K140" s="6">
+        <v>0</v>
+      </c>
+      <c r="L140">
+        <v>1.61</v>
+      </c>
+    </row>
+    <row r="141" spans="1:12">
+      <c r="A141" t="s">
+        <v>335</v>
+      </c>
+      <c r="B141" s="2">
+        <v>43224</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F141" s="6">
+        <v>14</v>
+      </c>
+      <c r="G141" s="6">
+        <v>14</v>
+      </c>
+      <c r="H141" s="6">
+        <v>7</v>
+      </c>
+      <c r="I141" s="6">
+        <v>7</v>
+      </c>
+      <c r="J141" s="6">
+        <v>0</v>
+      </c>
+      <c r="K141" s="6">
+        <v>0</v>
+      </c>
+      <c r="L141">
+        <v>1.37</v>
+      </c>
+    </row>
+    <row r="142" spans="1:12">
+      <c r="B142" s="2"/>
+    </row>
+    <row r="143" spans="1:12">
+      <c r="B143" s="2"/>
+    </row>
+    <row r="144" spans="1:12">
+      <c r="B144" s="2"/>
+    </row>
+    <row r="145" spans="1:18">
+      <c r="B145" s="2"/>
+    </row>
+    <row r="146" spans="1:18">
+      <c r="B146" s="2"/>
+    </row>
+    <row r="147" spans="1:18">
+      <c r="B147" s="2"/>
+    </row>
+    <row r="148" spans="1:18">
+      <c r="B148" s="2"/>
+    </row>
+    <row r="149" spans="1:18">
+      <c r="B149" s="2"/>
+    </row>
+    <row r="150" spans="1:18">
+      <c r="B150" s="2"/>
+    </row>
+    <row r="151" spans="1:18">
+      <c r="B151" s="2"/>
+    </row>
+    <row r="152" spans="1:18">
+      <c r="B152" s="2"/>
+    </row>
+    <row r="153" spans="1:18">
+      <c r="B153" s="2"/>
+    </row>
+    <row r="154" spans="1:18">
+      <c r="A154" s="3"/>
+      <c r="B154" s="5"/>
+      <c r="C154" s="4"/>
+      <c r="D154" s="3"/>
+      <c r="E154" s="4"/>
+      <c r="F154" s="7"/>
+      <c r="G154" s="7"/>
+      <c r="H154" s="7"/>
+      <c r="I154" s="7"/>
+      <c r="J154" s="7"/>
+      <c r="K154" s="7"/>
+      <c r="L154" s="3"/>
+      <c r="M154" s="3"/>
+      <c r="N154" s="3"/>
+      <c r="O154" s="3"/>
+      <c r="P154" s="3"/>
+      <c r="Q154" s="3"/>
+      <c r="R154" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>